<commit_message>
update cas d'usage et scenario d'utilisation
</commit_message>
<xml_diff>
--- a/Gestion_A_jmd.xlsx
+++ b/Gestion_A_jmd.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cvmqc-my.sharepoint.com/personal/e_ldilion_etu_cvm_qc_ca/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irvan PC\Documents\ecole\DEC\2023 - automne\GÉNIE LOGICIEL 1\ProjetDaleks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{235565F7-C2FF-4BF8-9439-9B3205FDF89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5826D61B-05A8-4F6F-A288-D7D957A32706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Méthodes SCRUM" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="250">
   <si>
     <t>Chiffrier de documentation de projets</t>
   </si>
@@ -341,18 +341,12 @@
     <t>air de jeu</t>
   </si>
   <si>
-    <t>affiche</t>
-  </si>
-  <si>
     <t>colonne et rangées</t>
   </si>
   <si>
     <t>Dalek</t>
   </si>
   <si>
-    <t>S approcher du docteur</t>
-  </si>
-  <si>
     <t>coordonée x y</t>
   </si>
   <si>
@@ -362,27 +356,12 @@
     <t>se deplacer</t>
   </si>
   <si>
-    <t>Feraille</t>
-  </si>
-  <si>
     <t>collision</t>
   </si>
   <si>
-    <t>eliminer le docteur et créer des ferailles</t>
-  </si>
-  <si>
     <t>docteur dalek feraille</t>
   </si>
   <si>
-    <t>Dalek_detruit</t>
-  </si>
-  <si>
-    <t>donner 5 points</t>
-  </si>
-  <si>
-    <t>points_joueur</t>
-  </si>
-  <si>
     <t>Dalek-teleporter</t>
   </si>
   <si>
@@ -396,9 +375,6 @@
   </si>
   <si>
     <t>teleporter</t>
-  </si>
-  <si>
-    <t>niveau dalek</t>
   </si>
   <si>
     <t>zappeur</t>
@@ -425,9 +401,6 @@
 explicites mais
 jamais mentionné)</t>
     </r>
-  </si>
-  <si>
-    <t>score</t>
   </si>
   <si>
     <r>
@@ -568,9 +541,6 @@
     <t>choix d'option du menu</t>
   </si>
   <si>
-    <t>while choix existant</t>
-  </si>
-  <si>
     <t>lancer une partie</t>
   </si>
   <si>
@@ -583,9 +553,6 @@
     <t>partie mise en cours</t>
   </si>
   <si>
-    <t>partie_en_cours == True</t>
-  </si>
-  <si>
     <t>afficher_air_de_jeu</t>
   </si>
   <si>
@@ -604,18 +571,6 @@
     <t>deplacer le Docteur</t>
   </si>
   <si>
-    <t>changer l'emplacement du Docteur</t>
-  </si>
-  <si>
-    <t>while coord xy hors air de jeux or input &lt; 1</t>
-  </si>
-  <si>
-    <t>Dalek x et y +-1</t>
-  </si>
-  <si>
-    <t>for dalek in daleks: changer la pos du dalek</t>
-  </si>
-  <si>
     <t>Fin du cas d'usage</t>
   </si>
   <si>
@@ -833,6 +788,207 @@
   </si>
   <si>
     <t>mise en forme conditionelle</t>
+  </si>
+  <si>
+    <t>creer air de jeu</t>
+  </si>
+  <si>
+    <t>Vue</t>
+  </si>
+  <si>
+    <t>afficher air de jeux, afficher score, affciher daleks docteur ferraille</t>
+  </si>
+  <si>
+    <t>Partie</t>
+  </si>
+  <si>
+    <t>niveau,air de jeux, docteur,daleks,ferraile,</t>
+  </si>
+  <si>
+    <t>creer un niveau,reglementer la partie,enregistrer le score, Vérifier les conditions de victoire/défaite,Passer au niveau suivant</t>
+  </si>
+  <si>
+    <t>lancer programe</t>
+  </si>
+  <si>
+    <t>press choix jeux</t>
+  </si>
+  <si>
+    <t>while choix = choix_existant</t>
+  </si>
+  <si>
+    <t>facile,moyen,difficil</t>
+  </si>
+  <si>
+    <t>affiche les differents niveau</t>
+  </si>
+  <si>
+    <t>choisi le niveau</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partie initialiser avec ses attribut </t>
+  </si>
+  <si>
+    <t>attribut en fonction de son niveau(nombre daleks,type de teleporteur et de zappeur)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verifier choix mouvement </t>
+  </si>
+  <si>
+    <t>deplacer daleks</t>
+  </si>
+  <si>
+    <t>if mouvement existe(entre 1 et 9) and mouvement possible(reste dans l'air de jeux)</t>
+  </si>
+  <si>
+    <t>en fonction du docteur</t>
+  </si>
+  <si>
+    <t>verifier collision</t>
+  </si>
+  <si>
+    <t>collision daleks docteur</t>
+  </si>
+  <si>
+    <t>collision daleks daleks</t>
+  </si>
+  <si>
+    <t>collision daleks ferraile</t>
+  </si>
+  <si>
+    <t>if position_dacleks = postion_docteur si vrai fin de partie(perdu)</t>
+  </si>
+  <si>
+    <t>if position_dacleks = postion_ferraile si vrai -1 daleks, +5 score et si nb_daleks = 0 alors fin de partiefin de partie(gagné)</t>
+  </si>
+  <si>
+    <t>if position_dacleks = postion_daleks si vrai creer_une_ferraile = position collision , -2 daleks , +5score et si nb_daleks = 0 alors fin de partie(gagné)</t>
+  </si>
+  <si>
+    <t>deplace le joueur aleatoirement</t>
+  </si>
+  <si>
+    <t>deplacement en fonction du niveau le plus pres (facile 2 case distance,oridanaire 0 case distance, meme case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">verififier collision </t>
+  </si>
+  <si>
+    <t>zapper</t>
+  </si>
+  <si>
+    <t>air de jeux, docteur,daleks,,</t>
+  </si>
+  <si>
+    <t>niveau dalek,docteur,ferraille,air de jeux</t>
+  </si>
+  <si>
+    <t>verifier si daleks a proximité</t>
+  </si>
+  <si>
+    <t xml:space="preserve">for daleks in tous_les_daleks if daleks is next to docteur daleks-1 </t>
+  </si>
+  <si>
+    <t>S approcher du docteur , supprimer un daleck</t>
+  </si>
+  <si>
+    <t>creer une ferraile</t>
+  </si>
+  <si>
+    <t>ferraille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">si fin partie </t>
+  </si>
+  <si>
+    <t>fin de partie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">partie_en_cours == False </t>
+  </si>
+  <si>
+    <t>verifie la cause de la fin de la partie</t>
+  </si>
+  <si>
+    <t>if nb _daleks = 0 partiewin else partieloose</t>
+  </si>
+  <si>
+    <t>en fonction de si la partie est gagné ou perdu</t>
+  </si>
+  <si>
+    <t>Vu affiche l'ecran de fin de partie et le score</t>
+  </si>
+  <si>
+    <t>interacton quelquonque</t>
+  </si>
+  <si>
+    <t>pour leave l'ecran de fin de partie</t>
+  </si>
+  <si>
+    <t>affciher les differentes score</t>
+  </si>
+  <si>
+    <t>press choix score</t>
+  </si>
+  <si>
+    <t>while choix = choix_existant =t</t>
+  </si>
+  <si>
+    <t>while choix = choix_existant = z and if zapper &gt; 0</t>
+  </si>
+  <si>
+    <t>If choix == s ou  S</t>
+  </si>
+  <si>
+    <t>vue accede a score</t>
+  </si>
+  <si>
+    <t>affiche l'ensemble des partie déja realisé avec le nom du jours ainsi que son score</t>
+  </si>
+  <si>
+    <t>demande au joueur de rentrer son nom</t>
+  </si>
+  <si>
+    <t>le jouer ecrit son nom</t>
+  </si>
+  <si>
+    <t>creation ferraille</t>
+  </si>
+  <si>
+    <t>si ferraille creer</t>
+  </si>
+  <si>
+    <t>supprime daleks</t>
+  </si>
+  <si>
+    <t>si daleks supprimé</t>
+  </si>
+  <si>
+    <t>while partie_en_cours == True</t>
+  </si>
+  <si>
+    <t>plateau et toutes les entité qui le compose (docteur position defini au prealable ou aleatoire) (daleks placer aleatoirement0</t>
+  </si>
+  <si>
+    <t>et if  nb_daleks =0 fin de partie</t>
+  </si>
+  <si>
+    <t>quitter le programe</t>
+  </si>
+  <si>
+    <t>If choix == q ou  Q</t>
+  </si>
+  <si>
+    <t>press choix  quitter</t>
+  </si>
+  <si>
+    <t>sort de la fonction controle</t>
+  </si>
+  <si>
+    <t>fin de main</t>
+  </si>
+  <si>
+    <t>fin de l'execution du programme</t>
   </si>
 </sst>
 </file>
@@ -844,7 +1000,7 @@
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -936,6 +1092,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1539,7 +1700,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1804,6 +1965,11 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1825,6 +1991,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1840,7 +2007,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1875,7 +2041,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2180,7 +2346,7 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="6.42578125" customWidth="1"/>
@@ -2193,7 +2359,7 @@
     <col min="9" max="28" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="17.25" customHeight="1">
+    <row r="2" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2204,7 +2370,7 @@
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="2:8" ht="17.25" customHeight="1">
+    <row r="3" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
       <c r="D3" s="13"/>
@@ -2213,7 +2379,7 @@
       <c r="G3" s="13"/>
       <c r="H3" s="112"/>
     </row>
-    <row r="4" spans="2:8" ht="17.25" customHeight="1">
+    <row r="4" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="14" t="s">
         <v>1</v>
       </c>
@@ -2224,7 +2390,7 @@
       <c r="G4" s="110"/>
       <c r="H4" s="110"/>
     </row>
-    <row r="5" spans="2:8" ht="17.25" customHeight="1">
+    <row r="5" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="110"/>
       <c r="C5" s="110"/>
       <c r="D5" s="110"/>
@@ -2233,7 +2399,7 @@
       <c r="G5" s="110"/>
       <c r="H5" s="110"/>
     </row>
-    <row r="6" spans="2:8" ht="17.25" customHeight="1">
+    <row r="6" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="110"/>
       <c r="C6" s="110"/>
       <c r="D6" s="110"/>
@@ -2242,7 +2408,7 @@
       <c r="G6" s="110"/>
       <c r="H6" s="110"/>
     </row>
-    <row r="7" spans="2:8" ht="17.25" customHeight="1">
+    <row r="7" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
@@ -2255,7 +2421,7 @@
       <c r="G7" s="35"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="2:8" ht="17.25" customHeight="1">
+    <row r="8" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="6"/>
       <c r="C8" s="13"/>
       <c r="D8" s="5"/>
@@ -2266,7 +2432,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="2:8" ht="17.25" customHeight="1">
+    <row r="9" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="6"/>
       <c r="C9" s="13" t="s">
         <v>5</v>
@@ -2280,7 +2446,7 @@
       </c>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="2:8" ht="17.25" customHeight="1">
+    <row r="10" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="6"/>
       <c r="C10" s="13"/>
       <c r="D10" s="5"/>
@@ -2288,7 +2454,7 @@
       <c r="F10" s="6"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="2:8" ht="17.25" customHeight="1">
+    <row r="11" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
       <c r="C11" s="13" t="s">
         <v>8</v>
@@ -2305,7 +2471,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="2:8" ht="17.25" customHeight="1">
+    <row r="12" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="6"/>
       <c r="C12" s="13"/>
       <c r="D12" s="5"/>
@@ -2316,7 +2482,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="2:8" ht="17.25" customHeight="1">
+    <row r="13" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="6"/>
       <c r="C13" s="13" t="s">
         <v>13</v>
@@ -2330,7 +2496,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="2:8" ht="17.25" customHeight="1">
+    <row r="14" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="6"/>
       <c r="C14" s="13"/>
       <c r="D14" s="5"/>
@@ -2340,7 +2506,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:8" ht="17.25" customHeight="1">
+    <row r="15" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="6"/>
       <c r="C15" s="13" t="s">
         <v>17</v>
@@ -2354,7 +2520,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="17.25" customHeight="1">
+    <row r="16" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="38"/>
       <c r="C16" s="112"/>
       <c r="D16" s="8" t="s">
@@ -2366,7 +2532,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="17.25" customHeight="1">
+    <row r="18" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="38"/>
       <c r="C18" s="112" t="s">
         <v>22</v>
@@ -2383,7 +2549,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:8" ht="17.25" customHeight="1">
+    <row r="19" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="38"/>
       <c r="C19" s="112"/>
       <c r="D19" s="8" t="s">
@@ -2396,7 +2562,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="2:8" ht="17.25" customHeight="1">
+    <row r="20" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="38"/>
       <c r="C20" s="112"/>
       <c r="D20" s="8"/>
@@ -2406,7 +2572,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="2:8" ht="17.25" customHeight="1">
+    <row r="21" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="38"/>
       <c r="C21" s="112" t="s">
         <v>29</v>
@@ -2420,7 +2586,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="2:8" ht="17.25" customHeight="1">
+    <row r="22" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="38"/>
       <c r="C22" s="112"/>
       <c r="D22" s="8" t="s">
@@ -2432,7 +2598,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="17.25" customHeight="1">
+    <row r="23" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="38"/>
       <c r="C23" s="112"/>
       <c r="D23" s="8"/>
@@ -2443,7 +2609,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="2:8" ht="17.25" customHeight="1">
+    <row r="24" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="38"/>
       <c r="C24" s="112" t="s">
         <v>35</v>
@@ -2457,7 +2623,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="2:8" ht="17.25" customHeight="1">
+    <row r="25" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="38"/>
       <c r="C25" s="112"/>
       <c r="D25" s="8" t="s">
@@ -2467,7 +2633,7 @@
       <c r="F25" s="38"/>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="2:8" ht="17.25" customHeight="1">
+    <row r="26" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B26" s="38"/>
       <c r="C26" s="110"/>
       <c r="D26" s="8"/>
@@ -2480,7 +2646,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="2:8" ht="17.25" customHeight="1">
+    <row r="27" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B27" s="38"/>
       <c r="C27" s="110"/>
       <c r="D27" s="8"/>
@@ -2490,7 +2656,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="2:8" ht="17.25" customHeight="1">
+    <row r="28" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="101" t="s">
         <v>42</v>
       </c>
@@ -2504,7 +2670,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="2:8" ht="17.25" customHeight="1">
+    <row r="29" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>45</v>
       </c>
@@ -2517,7 +2683,7 @@
       <c r="G29" s="112"/>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="2:8" ht="17.25" customHeight="1">
+    <row r="30" spans="2:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B30" s="38"/>
       <c r="C30" s="110"/>
       <c r="D30" s="12" t="s">
@@ -2532,89 +2698,89 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F36" s="134"/>
-      <c r="G36" s="135"/>
-      <c r="H36" s="135"/>
-      <c r="I36" s="135"/>
-    </row>
-    <row r="37" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F37" s="135"/>
-      <c r="G37" s="135"/>
-      <c r="H37" s="135"/>
-      <c r="I37" s="135"/>
-    </row>
-    <row r="38" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F38" s="135"/>
-      <c r="G38" s="135"/>
-      <c r="H38" s="135"/>
-      <c r="I38" s="135"/>
-    </row>
-    <row r="39" spans="6:9" ht="17.25" customHeight="1">
+    <row r="36" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F36" s="139"/>
+      <c r="G36" s="140"/>
+      <c r="H36" s="140"/>
+      <c r="I36" s="140"/>
+    </row>
+    <row r="37" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F37" s="140"/>
+      <c r="G37" s="140"/>
+      <c r="H37" s="140"/>
+      <c r="I37" s="140"/>
+    </row>
+    <row r="38" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F38" s="140"/>
+      <c r="G38" s="140"/>
+      <c r="H38" s="140"/>
+      <c r="I38" s="140"/>
+    </row>
+    <row r="39" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F39" s="112"/>
       <c r="G39" s="112"/>
       <c r="H39" s="112"/>
       <c r="I39" s="112"/>
     </row>
-    <row r="40" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F40" s="134"/>
-      <c r="G40" s="135"/>
-      <c r="H40" s="135"/>
-      <c r="I40" s="135"/>
-    </row>
-    <row r="41" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F41" s="135"/>
-      <c r="G41" s="135"/>
-      <c r="H41" s="135"/>
-      <c r="I41" s="135"/>
-    </row>
-    <row r="42" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F42" s="135"/>
-      <c r="G42" s="135"/>
-      <c r="H42" s="135"/>
-      <c r="I42" s="135"/>
-    </row>
-    <row r="43" spans="6:9" ht="17.25" customHeight="1">
+    <row r="40" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F40" s="139"/>
+      <c r="G40" s="140"/>
+      <c r="H40" s="140"/>
+      <c r="I40" s="140"/>
+    </row>
+    <row r="41" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F41" s="140"/>
+      <c r="G41" s="140"/>
+      <c r="H41" s="140"/>
+      <c r="I41" s="140"/>
+    </row>
+    <row r="42" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F42" s="140"/>
+      <c r="G42" s="140"/>
+      <c r="H42" s="140"/>
+      <c r="I42" s="140"/>
+    </row>
+    <row r="43" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F43" s="112"/>
       <c r="G43" s="112"/>
       <c r="H43" s="112"/>
       <c r="I43" s="112"/>
     </row>
-    <row r="44" spans="6:9" ht="17.25" customHeight="1">
+    <row r="44" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F44" s="112"/>
       <c r="G44" s="112"/>
       <c r="H44" s="112"/>
       <c r="I44" s="112"/>
     </row>
-    <row r="45" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F45" s="134"/>
-      <c r="G45" s="135"/>
-      <c r="H45" s="135"/>
-      <c r="I45" s="135"/>
-    </row>
-    <row r="46" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F46" s="135"/>
-      <c r="G46" s="135"/>
-      <c r="H46" s="135"/>
-      <c r="I46" s="135"/>
-    </row>
-    <row r="47" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F47" s="135"/>
-      <c r="G47" s="135"/>
-      <c r="H47" s="135"/>
-      <c r="I47" s="135"/>
-    </row>
-    <row r="48" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F48" s="135"/>
-      <c r="G48" s="135"/>
-      <c r="H48" s="135"/>
-      <c r="I48" s="135"/>
-    </row>
-    <row r="49" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F49" s="135"/>
-      <c r="G49" s="135"/>
-      <c r="H49" s="135"/>
-      <c r="I49" s="135"/>
+    <row r="45" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F45" s="139"/>
+      <c r="G45" s="140"/>
+      <c r="H45" s="140"/>
+      <c r="I45" s="140"/>
+    </row>
+    <row r="46" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F46" s="140"/>
+      <c r="G46" s="140"/>
+      <c r="H46" s="140"/>
+      <c r="I46" s="140"/>
+    </row>
+    <row r="47" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F47" s="140"/>
+      <c r="G47" s="140"/>
+      <c r="H47" s="140"/>
+      <c r="I47" s="140"/>
+    </row>
+    <row r="48" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F48" s="140"/>
+      <c r="G48" s="140"/>
+      <c r="H48" s="140"/>
+      <c r="I48" s="140"/>
+    </row>
+    <row r="49" spans="6:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F49" s="140"/>
+      <c r="G49" s="140"/>
+      <c r="H49" s="140"/>
+      <c r="I49" s="140"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2634,20 +2800,20 @@
   <dimension ref="B2:E40"/>
   <sheetViews>
     <sheetView zoomScale="63" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.85546875" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
     <col min="3" max="3" width="37.28515625" customWidth="1"/>
-    <col min="4" max="4" width="52.140625" customWidth="1"/>
-    <col min="5" max="5" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="138.7109375" customWidth="1"/>
+    <col min="5" max="5" width="48" customWidth="1"/>
     <col min="6" max="7" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="12.75" customHeight="1">
+    <row r="2" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="112"/>
       <c r="C2" s="14" t="s">
         <v>8</v>
@@ -2655,13 +2821,13 @@
       <c r="D2" s="112"/>
       <c r="E2" s="112"/>
     </row>
-    <row r="3" spans="2:5" ht="12.75" customHeight="1">
+    <row r="3" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="112"/>
       <c r="C3" s="110"/>
       <c r="D3" s="112"/>
       <c r="E3" s="112"/>
     </row>
-    <row r="4" spans="2:5" ht="12.75" customHeight="1">
+    <row r="4" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="112"/>
       <c r="C4" s="112" t="s">
         <v>50</v>
@@ -2669,7 +2835,7 @@
       <c r="D4" s="112"/>
       <c r="E4" s="112"/>
     </row>
-    <row r="5" spans="2:5" ht="12.75" customHeight="1">
+    <row r="5" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="112"/>
       <c r="C5" s="112" t="s">
         <v>51</v>
@@ -2677,7 +2843,7 @@
       <c r="D5" s="112"/>
       <c r="E5" s="112"/>
     </row>
-    <row r="6" spans="2:5" ht="12.75" customHeight="1">
+    <row r="6" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="112"/>
       <c r="C6" s="112" t="s">
         <v>52</v>
@@ -2685,7 +2851,7 @@
       <c r="D6" s="112"/>
       <c r="E6" s="112"/>
     </row>
-    <row r="7" spans="2:5" ht="12.75" customHeight="1">
+    <row r="7" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="112"/>
       <c r="C7" s="112" t="s">
         <v>53</v>
@@ -2693,7 +2859,7 @@
       <c r="D7" s="112"/>
       <c r="E7" s="112"/>
     </row>
-    <row r="8" spans="2:5" ht="12.75" customHeight="1">
+    <row r="8" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="112"/>
       <c r="C8" s="112" t="s">
         <v>54</v>
@@ -2701,7 +2867,7 @@
       <c r="D8" s="112"/>
       <c r="E8" s="112"/>
     </row>
-    <row r="9" spans="2:5" ht="15.75" customHeight="1">
+    <row r="9" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="112"/>
       <c r="C9" s="112" t="s">
         <v>55</v>
@@ -2709,7 +2875,7 @@
       <c r="D9" s="112"/>
       <c r="E9" s="112"/>
     </row>
-    <row r="10" spans="2:5" ht="15.75" customHeight="1">
+    <row r="10" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="112"/>
       <c r="C10" s="112" t="s">
         <v>56</v>
@@ -2717,13 +2883,13 @@
       <c r="D10" s="112"/>
       <c r="E10" s="112"/>
     </row>
-    <row r="11" spans="2:5" ht="15.75" customHeight="1">
+    <row r="11" spans="2:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="112"/>
       <c r="C11" s="112"/>
       <c r="D11" s="112"/>
       <c r="E11" s="112"/>
     </row>
-    <row r="12" spans="2:5" ht="12.75" customHeight="1">
+    <row r="12" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="14"/>
       <c r="C12" s="15" t="s">
         <v>57</v>
@@ -2735,230 +2901,236 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B13" s="136" t="s">
+    <row r="13" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="141" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="16" t="s">
         <v>61</v>
       </c>
       <c r="D13" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="E13" s="37" t="s">
         <v>62</v>
       </c>
-      <c r="E13" s="37" t="s">
+    </row>
+    <row r="14" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="142"/>
+      <c r="C14" s="22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="14" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B14" s="137"/>
-      <c r="C14" s="22" t="s">
+      <c r="D14" s="137" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="18" t="s">
+    </row>
+    <row r="15" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="142"/>
+      <c r="C15" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="D15" s="18" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="15" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B15" s="137"/>
-      <c r="C15" s="22" t="s">
+      <c r="E15" s="41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="142"/>
+      <c r="C16" s="138" t="s">
+        <v>218</v>
+      </c>
+      <c r="D16" s="137" t="s">
+        <v>217</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="142"/>
+      <c r="C17" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D17" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="E15" s="41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B16" s="137"/>
-      <c r="C16" s="22" t="s">
+    </row>
+    <row r="18" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="142"/>
+      <c r="C18" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="E18" s="41"/>
+    </row>
+    <row r="19" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="142"/>
+      <c r="C19" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B17" s="137"/>
-      <c r="C17" s="22" t="s">
+      <c r="D19" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="E19" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="E17" s="41" t="s">
+    </row>
+    <row r="20" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="142"/>
+      <c r="C20" s="22" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B18" s="137"/>
-      <c r="C18" s="22" t="s">
+      <c r="D20" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="E20" s="136" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="143"/>
+      <c r="C21" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="D21" s="40" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B19" s="137"/>
-      <c r="C19" s="22" t="s">
+      <c r="E21" s="135" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="141" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="E19" s="41" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B20" s="137"/>
-      <c r="C20" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="41" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B21" s="138"/>
-      <c r="C21" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D21" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" s="20"/>
-    </row>
-    <row r="22" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B22" s="136" t="s">
-        <v>84</v>
-      </c>
       <c r="C22" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="39"/>
-      <c r="E22" s="21"/>
-    </row>
-    <row r="23" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B23" s="137"/>
+        <v>186</v>
+      </c>
+      <c r="D22" s="39" t="s">
+        <v>188</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="142"/>
       <c r="C23" s="22"/>
       <c r="D23" s="18"/>
       <c r="E23" s="41"/>
     </row>
-    <row r="24" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B24" s="137"/>
+    <row r="24" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="142"/>
       <c r="C24" s="22"/>
       <c r="D24" s="18"/>
       <c r="E24" s="41"/>
     </row>
-    <row r="25" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B25" s="137"/>
+    <row r="25" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="142"/>
       <c r="C25" s="22"/>
       <c r="D25" s="18"/>
       <c r="E25" s="41"/>
     </row>
-    <row r="26" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B26" s="137"/>
+    <row r="26" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="142"/>
       <c r="C26" s="22"/>
       <c r="D26" s="18"/>
       <c r="E26" s="41"/>
     </row>
-    <row r="27" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B27" s="137"/>
+    <row r="27" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="142"/>
       <c r="C27" s="22"/>
       <c r="D27" s="18"/>
       <c r="E27" s="41"/>
     </row>
-    <row r="28" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B28" s="137"/>
+    <row r="28" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="142"/>
       <c r="C28" s="22"/>
       <c r="D28" s="18"/>
       <c r="E28" s="41"/>
     </row>
-    <row r="29" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B29" s="137"/>
+    <row r="29" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="142"/>
       <c r="C29" s="22"/>
       <c r="D29" s="18"/>
       <c r="E29" s="41"/>
     </row>
-    <row r="30" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B30" s="138"/>
+    <row r="30" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="143"/>
       <c r="C30" s="19"/>
       <c r="D30" s="40"/>
       <c r="E30" s="20"/>
     </row>
-    <row r="31" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B31" s="136" t="s">
-        <v>86</v>
+    <row r="31" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="141" t="s">
+        <v>77</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D31" s="39"/>
       <c r="E31" s="21"/>
     </row>
-    <row r="32" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B32" s="137"/>
+    <row r="32" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="142"/>
       <c r="C32" s="22"/>
       <c r="D32" s="18"/>
       <c r="E32" s="41"/>
     </row>
-    <row r="33" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B33" s="137"/>
+    <row r="33" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="142"/>
       <c r="C33" s="22"/>
       <c r="D33" s="18"/>
       <c r="E33" s="41"/>
     </row>
-    <row r="34" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B34" s="137"/>
+    <row r="34" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="142"/>
       <c r="C34" s="22"/>
       <c r="D34" s="18"/>
       <c r="E34" s="41"/>
     </row>
-    <row r="35" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B35" s="137"/>
+    <row r="35" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="142"/>
       <c r="C35" s="22"/>
       <c r="D35" s="18"/>
       <c r="E35" s="41"/>
     </row>
-    <row r="36" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B36" s="137"/>
+    <row r="36" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="142"/>
       <c r="C36" s="22"/>
       <c r="D36" s="18"/>
       <c r="E36" s="41"/>
     </row>
-    <row r="37" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B37" s="137"/>
+    <row r="37" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="142"/>
       <c r="C37" s="22"/>
       <c r="D37" s="18"/>
       <c r="E37" s="41"/>
     </row>
-    <row r="38" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B38" s="137"/>
+    <row r="38" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="142"/>
       <c r="C38" s="22"/>
       <c r="D38" s="18"/>
       <c r="E38" s="41"/>
     </row>
-    <row r="39" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B39" s="137"/>
+    <row r="39" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="142"/>
       <c r="C39" s="22"/>
       <c r="D39" s="18"/>
       <c r="E39" s="41"/>
     </row>
-    <row r="40" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B40" s="138"/>
+    <row r="40" spans="2:5" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="143"/>
       <c r="C40" s="24"/>
       <c r="D40" s="25"/>
       <c r="E40" s="46"/>
@@ -2978,244 +3150,596 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:F82"/>
+  <dimension ref="B2:F105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="94" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="C47" zoomScale="94" workbookViewId="0">
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
     <col min="4" max="4" width="44.42578125" customWidth="1"/>
     <col min="5" max="5" width="49.5703125" customWidth="1"/>
-    <col min="6" max="6" width="70.7109375" customWidth="1"/>
+    <col min="6" max="6" width="138.7109375" customWidth="1"/>
     <col min="7" max="8" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" ht="20.25" customHeight="1">
+    <row r="2" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="109"/>
       <c r="C2" s="28" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D2" s="109"/>
       <c r="E2" s="109"/>
       <c r="F2" s="109"/>
     </row>
-    <row r="3" spans="2:6" ht="89.45" customHeight="1">
+    <row r="3" spans="2:6" ht="89.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="109"/>
-      <c r="C3" s="139" t="s">
-        <v>89</v>
-      </c>
-      <c r="D3" s="135"/>
-      <c r="E3" s="135"/>
+      <c r="C3" s="144" t="s">
+        <v>80</v>
+      </c>
+      <c r="D3" s="140"/>
+      <c r="E3" s="140"/>
       <c r="F3" s="109"/>
     </row>
-    <row r="4" spans="2:6" ht="30.75" customHeight="1">
+    <row r="4" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="110"/>
-      <c r="C4" s="140" t="s">
-        <v>90</v>
-      </c>
-      <c r="D4" s="135"/>
-      <c r="E4" s="135"/>
+      <c r="C4" s="145" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="140"/>
+      <c r="E4" s="140"/>
       <c r="F4" s="110"/>
     </row>
-    <row r="5" spans="2:6" ht="21" customHeight="1">
+    <row r="5" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="109"/>
       <c r="C5" s="26" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="D5" s="109"/>
       <c r="E5" s="109"/>
       <c r="F5" s="109"/>
     </row>
-    <row r="6" spans="2:6" ht="21" customHeight="1">
+    <row r="6" spans="2:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="110"/>
       <c r="C6" s="27" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="D6" s="112"/>
       <c r="E6" s="112"/>
       <c r="F6" s="110"/>
     </row>
-    <row r="7" spans="2:6" ht="18" customHeight="1">
+    <row r="7" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="110"/>
       <c r="C7" s="112"/>
       <c r="D7" s="112"/>
       <c r="E7" s="112"/>
       <c r="F7" s="110"/>
     </row>
-    <row r="8" spans="2:6" ht="18" customHeight="1">
+    <row r="8" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
       <c r="E8" s="110"/>
       <c r="F8" s="28"/>
     </row>
-    <row r="9" spans="2:6" ht="19.5" customHeight="1">
+    <row r="9" spans="2:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="29" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D9" s="29" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="F9" s="29"/>
     </row>
-    <row r="10" spans="2:6" ht="18" customHeight="1">
+    <row r="10" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="110"/>
       <c r="C10" s="112"/>
       <c r="D10" s="110"/>
       <c r="E10" s="110"/>
       <c r="F10" s="110"/>
     </row>
-    <row r="11" spans="2:6" ht="18" customHeight="1">
+    <row r="11" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="28" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" ht="18" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="28"/>
       <c r="C12" s="14"/>
       <c r="D12" s="32"/>
     </row>
-    <row r="13" spans="2:6" ht="18" customHeight="1">
+    <row r="13" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>102</v>
-      </c>
-      <c r="C13" s="14"/>
+        <v>93</v>
+      </c>
+      <c r="C13" s="134" t="s">
+        <v>189</v>
+      </c>
       <c r="D13" s="132" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" ht="18" customHeight="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="110"/>
       <c r="C14" s="112"/>
       <c r="D14" s="110"/>
       <c r="E14" s="133" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" ht="18" customHeight="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="110"/>
       <c r="C15" s="32"/>
       <c r="D15" s="110"/>
       <c r="E15" s="133" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="F15" s="133"/>
     </row>
-    <row r="16" spans="2:6" ht="15.75" customHeight="1">
+    <row r="16" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E16" s="133" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="3:6" ht="15.75" customHeight="1">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D17" s="133"/>
       <c r="E17" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E18" s="133" t="s">
+        <v>99</v>
+      </c>
+      <c r="F18" s="133" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="133" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="133" t="s">
+        <v>190</v>
+      </c>
+      <c r="F19" s="133" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D20" s="133"/>
+      <c r="E20" s="133" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="133"/>
+    </row>
+    <row r="21" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D21" s="133"/>
+      <c r="E21" s="133" t="s">
+        <v>235</v>
+      </c>
+      <c r="F21" s="133"/>
+    </row>
+    <row r="22" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D22" s="133" t="s">
+        <v>236</v>
+      </c>
+      <c r="E22" s="133"/>
+      <c r="F22" s="133"/>
+    </row>
+    <row r="23" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D23" s="133"/>
+      <c r="E23" s="133" t="s">
+        <v>193</v>
+      </c>
+      <c r="F23" s="133" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="24" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D24" s="133" t="s">
+        <v>194</v>
+      </c>
+      <c r="E24" s="133"/>
+      <c r="F24" s="133"/>
+    </row>
+    <row r="25" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D25" s="133"/>
+      <c r="E25" s="133" t="s">
+        <v>195</v>
+      </c>
+      <c r="F25" s="133" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E26" s="133" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="133" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="27" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E27" s="133" t="s">
+        <v>104</v>
+      </c>
+      <c r="F27" s="133" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="28" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E28" s="133" t="s">
+        <v>105</v>
+      </c>
+      <c r="F28" s="133" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>106</v>
+      </c>
+      <c r="F29" s="133" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D30" s="133"/>
+      <c r="E30" s="133" t="s">
+        <v>197</v>
+      </c>
+      <c r="F30" s="133" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D31" s="133"/>
+      <c r="E31" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="133"/>
+    </row>
+    <row r="32" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D32" s="133"/>
+      <c r="E32" s="133" t="s">
+        <v>198</v>
+      </c>
+      <c r="F32" s="133" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C33" s="133" t="s">
+        <v>201</v>
+      </c>
+      <c r="E33" s="133" t="s">
+        <v>202</v>
+      </c>
+      <c r="F33" s="133" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E34" s="133" t="s">
+        <v>203</v>
+      </c>
+      <c r="F34" s="133" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="35" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E35" s="133" t="s">
+        <v>204</v>
+      </c>
+      <c r="F35" s="133" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="36" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E36" s="133" t="s">
+        <v>239</v>
+      </c>
+      <c r="F36" s="133" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="37" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E37" s="133" t="s">
+        <v>237</v>
+      </c>
+      <c r="F37" s="133" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="38" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E38" s="133" t="s">
+        <v>104</v>
+      </c>
+      <c r="F38" s="133"/>
+    </row>
+    <row r="39" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="133" t="s">
+        <v>73</v>
+      </c>
+      <c r="D39" s="133" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="18" spans="3:6" ht="15.75" customHeight="1">
-      <c r="D18" s="133" t="s">
-        <v>108</v>
-      </c>
-      <c r="F18" t="s">
+      <c r="F39" s="133" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="40" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E40" s="133" t="s">
+        <v>208</v>
+      </c>
+      <c r="F40" s="133" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="19" spans="3:6" ht="15.75" customHeight="1">
-      <c r="C19" t="s">
+      <c r="F41" s="133"/>
+    </row>
+    <row r="42" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" s="133" t="s">
+        <v>210</v>
+      </c>
+      <c r="E42" s="133" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C43" s="133"/>
+      <c r="E43" s="133" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="44" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C44" s="133"/>
+      <c r="E44" s="133" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="45" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C45" s="133"/>
+      <c r="E45" s="133" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="46" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C46" s="133"/>
+      <c r="E46" s="133" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="47" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C47" s="133"/>
+      <c r="E47" s="133" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C48" s="133" t="s">
+        <v>211</v>
+      </c>
+      <c r="D48" s="133" t="s">
+        <v>107</v>
+      </c>
+      <c r="F48" s="133" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E49" s="133" t="s">
+        <v>214</v>
+      </c>
+      <c r="F49" s="133" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E50" s="133" t="s">
+        <v>239</v>
+      </c>
+      <c r="F50" s="133" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="51" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E51" s="133" t="s">
+        <v>198</v>
+      </c>
+      <c r="F51" s="133"/>
+    </row>
+    <row r="52" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C52" s="133" t="s">
+        <v>201</v>
+      </c>
+      <c r="D52" s="112"/>
+      <c r="E52" s="133" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C53" s="133"/>
+      <c r="D53" s="112"/>
+      <c r="E53" s="133" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="54" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="133"/>
+      <c r="D54" s="112"/>
+      <c r="E54" s="133" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="55" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C55" s="133"/>
+      <c r="D55" s="112"/>
+      <c r="E55" s="133" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="56" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C56" s="133"/>
+      <c r="D56" s="112"/>
+      <c r="E56" s="133" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C57" s="133"/>
+      <c r="D57" s="112"/>
+      <c r="E57" s="133" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="58" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C58" s="133" t="s">
+        <v>220</v>
+      </c>
+      <c r="E58" s="133" t="s">
+        <v>219</v>
+      </c>
+      <c r="F58" s="133" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C59" s="133"/>
+      <c r="E59" s="133" t="s">
+        <v>222</v>
+      </c>
+      <c r="F59" s="133" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="60" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E60" s="133" t="s">
+        <v>225</v>
+      </c>
+      <c r="F60" s="133" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D61" s="133" t="s">
+        <v>226</v>
+      </c>
+      <c r="F61" s="133" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="62" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E62" s="133" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E63" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E64" s="133" t="s">
+        <v>99</v>
+      </c>
+      <c r="F64" s="133" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="65" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C65" s="133" t="s">
+        <v>228</v>
+      </c>
+      <c r="D65" s="133" t="s">
+        <v>229</v>
+      </c>
+      <c r="F65" s="133" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="66" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E66" s="133" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="67" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E67" s="133" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D68" s="133" t="s">
+        <v>226</v>
+      </c>
+      <c r="F68" s="133" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E69" s="133" t="s">
+        <v>99</v>
+      </c>
+      <c r="F69" s="133" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C70" s="133" t="s">
+        <v>244</v>
+      </c>
+      <c r="D70" s="133" t="s">
+        <v>246</v>
+      </c>
+      <c r="F70" s="133" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E71" s="133" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E72" s="133" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E73" s="133" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="105" spans="4:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D105" t="s">
         <v>110</v>
-      </c>
-      <c r="D19" s="133"/>
-      <c r="E19" s="133" t="s">
-        <v>111</v>
-      </c>
-      <c r="F19" s="133" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="3:6" ht="15.75" customHeight="1">
-      <c r="E20" s="133" t="s">
-        <v>113</v>
-      </c>
-      <c r="F20" s="133" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="3:6" ht="15.75" customHeight="1">
-      <c r="E21" s="133" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="3:6" ht="15.75" customHeight="1">
-      <c r="E22" s="133" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="3:6" ht="15.75" customHeight="1">
-      <c r="C23" t="s">
-        <v>117</v>
-      </c>
-      <c r="D23" s="133" t="s">
-        <v>118</v>
-      </c>
-      <c r="F23" s="133" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="24" spans="3:6" ht="15.75" customHeight="1">
-      <c r="D24" s="133"/>
-      <c r="F24" s="133"/>
-    </row>
-    <row r="25" spans="3:6" ht="15.75" customHeight="1">
-      <c r="D25" s="133"/>
-      <c r="E25" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="26" spans="3:6" ht="15.75" customHeight="1">
-      <c r="E26" s="133" t="s">
-        <v>121</v>
-      </c>
-      <c r="F26" s="133" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="27" spans="3:6" ht="15.75" customHeight="1">
-      <c r="E27" t="s">
-        <v>123</v>
-      </c>
-      <c r="F27" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" ht="18" customHeight="1">
-      <c r="D34" s="112"/>
-    </row>
-    <row r="82" spans="4:4" ht="15.75" customHeight="1">
-      <c r="D82" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -3237,14 +3761,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="101" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="7:19" ht="21.75" customHeight="1">
+    <row r="1" spans="7:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G1" s="14" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="H1" s="13"/>
       <c r="I1" s="13"/>
@@ -3259,9 +3783,9 @@
       <c r="R1" s="13"/>
       <c r="S1" s="13"/>
     </row>
-    <row r="2" spans="7:19" ht="15">
+    <row r="2" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G2" s="13" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="H2" s="112"/>
       <c r="I2" s="112"/>
@@ -3276,9 +3800,9 @@
       <c r="R2" s="112"/>
       <c r="S2" s="112"/>
     </row>
-    <row r="3" spans="7:19" ht="15">
+    <row r="3" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G3" s="33" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="H3" s="112"/>
       <c r="I3" s="112"/>
@@ -3293,7 +3817,7 @@
       <c r="R3" s="112"/>
       <c r="S3" s="112"/>
     </row>
-    <row r="4" spans="7:19" ht="15">
+    <row r="4" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G4" s="112"/>
       <c r="H4" s="112"/>
       <c r="I4" s="112"/>
@@ -3308,7 +3832,7 @@
       <c r="R4" s="112"/>
       <c r="S4" s="112"/>
     </row>
-    <row r="5" spans="7:19" ht="15">
+    <row r="5" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G5" s="112"/>
       <c r="H5" s="112"/>
       <c r="I5" s="112"/>
@@ -3323,9 +3847,9 @@
       <c r="R5" s="112"/>
       <c r="S5" s="112"/>
     </row>
-    <row r="6" spans="7:19" ht="15">
+    <row r="6" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G6" s="112" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="H6" s="112"/>
       <c r="I6" s="112"/>
@@ -3340,7 +3864,7 @@
       <c r="R6" s="112"/>
       <c r="S6" s="112"/>
     </row>
-    <row r="7" spans="7:19" ht="15">
+    <row r="7" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G7" s="112"/>
       <c r="H7" s="112"/>
       <c r="I7" s="112"/>
@@ -3355,9 +3879,9 @@
       <c r="R7" s="112"/>
       <c r="S7" s="112"/>
     </row>
-    <row r="8" spans="7:19" ht="15">
+    <row r="8" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G8" s="112" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="H8" s="112"/>
       <c r="I8" s="112"/>
@@ -3372,7 +3896,7 @@
       <c r="R8" s="112"/>
       <c r="S8" s="112"/>
     </row>
-    <row r="9" spans="7:19" ht="15">
+    <row r="9" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G9" s="112"/>
       <c r="H9" s="112"/>
       <c r="I9" s="112"/>
@@ -3387,7 +3911,7 @@
       <c r="R9" s="112"/>
       <c r="S9" s="112"/>
     </row>
-    <row r="10" spans="7:19" ht="15.6">
+    <row r="10" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G10" s="34"/>
       <c r="H10" s="35"/>
       <c r="I10" s="35"/>
@@ -3395,7 +3919,7 @@
       <c r="K10" s="35"/>
       <c r="L10" s="35"/>
       <c r="M10" s="36" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="N10" s="35"/>
       <c r="O10" s="35"/>
@@ -3404,31 +3928,31 @@
       <c r="R10" s="35"/>
       <c r="S10" s="37"/>
     </row>
-    <row r="11" spans="7:19" ht="15">
+    <row r="11" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G11" s="38"/>
       <c r="H11" s="112"/>
       <c r="I11" s="112"/>
       <c r="J11" s="112"/>
       <c r="K11" s="112"/>
       <c r="L11" s="112"/>
-      <c r="M11" s="141"/>
-      <c r="N11" s="135"/>
-      <c r="O11" s="135"/>
+      <c r="M11" s="147"/>
+      <c r="N11" s="140"/>
+      <c r="O11" s="140"/>
       <c r="P11" s="112"/>
       <c r="Q11" s="112"/>
-      <c r="R11" s="141"/>
-      <c r="S11" s="142"/>
-    </row>
-    <row r="12" spans="7:19" ht="15">
+      <c r="R11" s="147"/>
+      <c r="S11" s="148"/>
+    </row>
+    <row r="12" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G12" s="38"/>
       <c r="H12" s="112" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="I12" s="112"/>
       <c r="J12" s="112"/>
       <c r="K12" s="112"/>
       <c r="L12" s="42" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="M12" s="49"/>
       <c r="N12" s="49"/>
@@ -3438,7 +3962,7 @@
       <c r="R12" s="39"/>
       <c r="S12" s="41"/>
     </row>
-    <row r="13" spans="7:19" ht="15">
+    <row r="13" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G13" s="38"/>
       <c r="H13" s="112"/>
       <c r="I13" s="112"/>
@@ -3453,7 +3977,7 @@
       <c r="R13" s="40"/>
       <c r="S13" s="41"/>
     </row>
-    <row r="14" spans="7:19" ht="15">
+    <row r="14" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G14" s="38"/>
       <c r="H14" s="112"/>
       <c r="I14" s="112"/>
@@ -3468,16 +3992,16 @@
       <c r="R14" s="112"/>
       <c r="S14" s="41"/>
     </row>
-    <row r="15" spans="7:19" ht="15">
+    <row r="15" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G15" s="38"/>
       <c r="H15" s="112" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="I15" s="112"/>
       <c r="J15" s="112"/>
       <c r="K15" s="112"/>
       <c r="L15" s="42" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="M15" s="49"/>
       <c r="N15" s="49"/>
@@ -3487,10 +4011,10 @@
       <c r="R15" s="39"/>
       <c r="S15" s="41"/>
     </row>
-    <row r="16" spans="7:19" ht="15">
+    <row r="16" spans="7:19" ht="15" x14ac:dyDescent="0.2">
       <c r="G16" s="38"/>
       <c r="H16" s="112" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="I16" s="112"/>
       <c r="J16" s="112"/>
@@ -3504,12 +4028,12 @@
       <c r="R16" s="40"/>
       <c r="S16" s="41"/>
     </row>
-    <row r="18" spans="7:23" ht="15.6">
+    <row r="18" spans="7:23" ht="15" x14ac:dyDescent="0.2">
       <c r="G18" s="38"/>
       <c r="H18" s="42"/>
       <c r="I18" s="49"/>
       <c r="J18" s="43" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="K18" s="49"/>
       <c r="L18" s="39"/>
@@ -3517,7 +4041,7 @@
       <c r="N18" s="42"/>
       <c r="O18" s="49"/>
       <c r="P18" s="43" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="Q18" s="49"/>
       <c r="R18" s="39"/>
@@ -3527,7 +4051,7 @@
       <c r="V18" s="112"/>
       <c r="W18" s="112"/>
     </row>
-    <row r="19" spans="7:23" ht="15">
+    <row r="19" spans="7:23" ht="15" x14ac:dyDescent="0.2">
       <c r="G19" s="38"/>
       <c r="H19" s="53"/>
       <c r="I19" s="54"/>
@@ -3546,7 +4070,7 @@
       <c r="V19" s="112"/>
       <c r="W19" s="112"/>
     </row>
-    <row r="20" spans="7:23" ht="15">
+    <row r="20" spans="7:23" ht="15" x14ac:dyDescent="0.2">
       <c r="G20" s="44"/>
       <c r="H20" s="45"/>
       <c r="I20" s="45"/>
@@ -3565,7 +4089,7 @@
       <c r="V20" s="112"/>
       <c r="W20" s="112"/>
     </row>
-    <row r="21" spans="7:23" ht="15">
+    <row r="21" spans="7:23" ht="15" x14ac:dyDescent="0.2">
       <c r="G21" s="112"/>
       <c r="H21" s="112"/>
       <c r="I21" s="112"/>
@@ -3584,7 +4108,7 @@
       <c r="V21" s="112"/>
       <c r="W21" s="112"/>
     </row>
-    <row r="22" spans="7:23" ht="15">
+    <row r="22" spans="7:23" ht="15" x14ac:dyDescent="0.2">
       <c r="G22" s="112"/>
       <c r="H22" s="112"/>
       <c r="I22" s="112"/>
@@ -3603,7 +4127,7 @@
       <c r="V22" s="112"/>
       <c r="W22" s="112"/>
     </row>
-    <row r="23" spans="7:23" ht="15">
+    <row r="23" spans="7:23" ht="15" x14ac:dyDescent="0.2">
       <c r="G23" s="112"/>
       <c r="H23" s="112"/>
       <c r="I23" s="112"/>
@@ -3622,10 +4146,10 @@
       <c r="V23" s="112"/>
       <c r="W23" s="112"/>
     </row>
-    <row r="24" spans="7:23" ht="15">
+    <row r="24" spans="7:23" ht="15" x14ac:dyDescent="0.2">
       <c r="G24" s="146"/>
-      <c r="H24" s="135"/>
-      <c r="I24" s="135"/>
+      <c r="H24" s="140"/>
+      <c r="I24" s="140"/>
       <c r="J24" s="112"/>
       <c r="K24" s="112"/>
       <c r="L24" s="112"/>
@@ -3641,7 +4165,7 @@
       <c r="V24" s="112"/>
       <c r="W24" s="112"/>
     </row>
-    <row r="25" spans="7:23" ht="15">
+    <row r="25" spans="7:23" ht="15" x14ac:dyDescent="0.2">
       <c r="G25" s="112"/>
       <c r="H25" s="112"/>
       <c r="I25" s="112"/>
@@ -3660,10 +4184,10 @@
       <c r="V25" s="112"/>
       <c r="W25" s="112"/>
     </row>
-    <row r="26" spans="7:23" ht="15">
+    <row r="26" spans="7:23" ht="15" x14ac:dyDescent="0.2">
       <c r="G26" s="146"/>
-      <c r="H26" s="135"/>
-      <c r="I26" s="135"/>
+      <c r="H26" s="140"/>
+      <c r="I26" s="140"/>
       <c r="J26" s="112"/>
       <c r="K26" s="112"/>
       <c r="L26" s="112"/>
@@ -3679,7 +4203,7 @@
       <c r="V26" s="112"/>
       <c r="W26" s="112"/>
     </row>
-    <row r="27" spans="7:23" ht="15">
+    <row r="27" spans="7:23" ht="15" x14ac:dyDescent="0.2">
       <c r="G27" s="112"/>
       <c r="H27" s="112"/>
       <c r="I27" s="112"/>
@@ -3698,7 +4222,7 @@
       <c r="V27" s="112"/>
       <c r="W27" s="112"/>
     </row>
-    <row r="28" spans="7:23" ht="15">
+    <row r="28" spans="7:23" ht="15" x14ac:dyDescent="0.2">
       <c r="G28" s="112"/>
       <c r="H28" s="112"/>
       <c r="I28" s="112"/>
@@ -3709,13 +4233,13 @@
       <c r="N28" s="112"/>
       <c r="O28" s="112"/>
       <c r="P28" s="146"/>
-      <c r="Q28" s="135"/>
-      <c r="R28" s="135"/>
+      <c r="Q28" s="140"/>
+      <c r="R28" s="140"/>
       <c r="S28" s="112"/>
       <c r="T28" s="146"/>
-      <c r="U28" s="135"/>
-      <c r="V28" s="135"/>
-      <c r="W28" s="135"/>
+      <c r="U28" s="140"/>
+      <c r="V28" s="140"/>
+      <c r="W28" s="140"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3739,7 +4263,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -3755,18 +4279,18 @@
     <col min="12" max="30" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="87" customHeight="1">
+    <row r="1" spans="2:8" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="110"/>
-      <c r="C1" s="139" t="s">
-        <v>139</v>
-      </c>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-    </row>
-    <row r="2" spans="2:8" ht="12.75" customHeight="1">
+      <c r="C1" s="144" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+    </row>
+    <row r="2" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="112"/>
       <c r="C2" s="112"/>
       <c r="D2" s="112"/>
@@ -3775,9 +4299,9 @@
       <c r="G2" s="112"/>
       <c r="H2" s="112"/>
     </row>
-    <row r="3" spans="2:8" ht="12.75" customHeight="1">
+    <row r="3" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="14" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="C3" s="112"/>
       <c r="D3" s="47"/>
@@ -3786,7 +4310,7 @@
       <c r="G3" s="47"/>
       <c r="H3" s="47"/>
     </row>
-    <row r="4" spans="2:8" ht="18" customHeight="1">
+    <row r="4" spans="2:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="112"/>
       <c r="C4" s="47"/>
       <c r="D4" s="47"/>
@@ -3795,10 +4319,10 @@
       <c r="G4" s="47"/>
       <c r="H4" s="47"/>
     </row>
-    <row r="5" spans="2:8" ht="15" customHeight="1">
+    <row r="5" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="112"/>
       <c r="C5" s="47" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="D5" s="47"/>
       <c r="E5" s="47"/>
@@ -3806,7 +4330,7 @@
       <c r="G5" s="47"/>
       <c r="H5" s="112"/>
     </row>
-    <row r="6" spans="2:8" ht="12.75" customHeight="1">
+    <row r="6" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="110"/>
       <c r="C6" s="110"/>
       <c r="D6" s="110"/>
@@ -3815,31 +4339,31 @@
       <c r="G6" s="112"/>
       <c r="H6" s="110"/>
     </row>
-    <row r="7" spans="2:8" ht="12.75" customHeight="1">
+    <row r="7" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="110"/>
       <c r="C7" s="110"/>
       <c r="D7" s="48" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="E7" s="49"/>
       <c r="F7" s="49"/>
       <c r="G7" s="50" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="H7" s="110"/>
     </row>
-    <row r="8" spans="2:8" ht="12.75" customHeight="1">
+    <row r="8" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="110"/>
       <c r="C8" s="110"/>
       <c r="D8" s="51" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="E8" s="112"/>
       <c r="F8" s="112"/>
       <c r="G8" s="52"/>
       <c r="H8" s="110"/>
     </row>
-    <row r="9" spans="2:8" ht="12.75" customHeight="1">
+    <row r="9" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="110"/>
       <c r="C9" s="110"/>
       <c r="D9" s="53"/>
@@ -3848,15 +4372,15 @@
       <c r="G9" s="52"/>
       <c r="H9" s="110"/>
     </row>
-    <row r="10" spans="2:8" ht="12.75" customHeight="1">
+    <row r="10" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="110"/>
       <c r="C10" s="110"/>
       <c r="D10" s="55" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="E10" s="112"/>
       <c r="F10" s="112" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="G10" s="52"/>
       <c r="H10" s="110"/>
@@ -3878,7 +4402,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="5" width="17" customWidth="1"/>
@@ -3886,112 +4410,112 @@
     <col min="7" max="26" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="64.5" customHeight="1">
-      <c r="C1" s="143" t="s">
-        <v>147</v>
-      </c>
-      <c r="D1" s="135"/>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-    </row>
-    <row r="2" spans="2:11" ht="13.15"/>
-    <row r="3" spans="2:11" ht="13.15">
+    <row r="1" spans="2:11" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C1" s="149" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="140"/>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+    </row>
+    <row r="2" spans="2:11" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="3" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B3" s="56" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="2:11" ht="13.15">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B4" s="57"/>
     </row>
-    <row r="5" spans="2:11" ht="13.15">
+    <row r="5" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="113"/>
       <c r="C5" s="113"/>
       <c r="D5" s="113"/>
     </row>
-    <row r="6" spans="2:11" ht="13.15">
+    <row r="6" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B6" s="113"/>
       <c r="C6" s="113"/>
       <c r="D6" s="113"/>
       <c r="E6" s="113"/>
     </row>
-    <row r="7" spans="2:11" ht="26.45">
-      <c r="B7" s="144" t="s">
-        <v>149</v>
-      </c>
-      <c r="C7" s="135"/>
+    <row r="7" spans="2:11" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="B7" s="150" t="s">
+        <v>134</v>
+      </c>
+      <c r="C7" s="140"/>
       <c r="G7" s="113" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="H7" s="113"/>
       <c r="I7" s="113"/>
       <c r="J7" s="113"/>
     </row>
-    <row r="8" spans="2:11" ht="13.15">
+    <row r="8" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B8" s="113"/>
       <c r="G8" s="113" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="H8" s="113"/>
       <c r="I8" s="113"/>
     </row>
-    <row r="9" spans="2:11" ht="13.15">
+    <row r="9" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B9" s="58" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="C9" s="59" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="D9" s="60" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="G9" s="61"/>
       <c r="H9" s="62" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="I9" s="62" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="J9" s="62" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="K9" s="63" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="10" spans="2:11" ht="13.15">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B10" s="108"/>
       <c r="D10" s="67"/>
       <c r="G10" s="68" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="J10" s="113"/>
       <c r="K10" s="111"/>
     </row>
-    <row r="11" spans="2:11" ht="26.45">
+    <row r="11" spans="2:11" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B11" s="64"/>
       <c r="C11" s="65"/>
       <c r="D11" s="66"/>
       <c r="E11" s="113" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="G11" s="68" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="K11" s="111"/>
     </row>
-    <row r="12" spans="2:11" ht="13.15">
+    <row r="12" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B12" s="108"/>
       <c r="D12" s="67"/>
       <c r="G12" s="68" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="K12" s="111"/>
     </row>
-    <row r="13" spans="2:11" ht="13.15">
+    <row r="13" spans="2:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B13" s="108"/>
       <c r="D13" s="67"/>
       <c r="G13" s="68" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="K13" s="111"/>
     </row>
@@ -4015,7 +4539,7 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" customWidth="1"/>
@@ -4026,18 +4550,18 @@
     <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="57" customHeight="1">
+    <row r="1" spans="2:8" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="115"/>
       <c r="C1" s="116"/>
-      <c r="D1" s="143" t="s">
-        <v>163</v>
-      </c>
-      <c r="E1" s="135"/>
-      <c r="F1" s="135"/>
-      <c r="G1" s="135"/>
-      <c r="H1" s="135"/>
-    </row>
-    <row r="2" spans="2:8" ht="12.75" customHeight="1">
+      <c r="D1" s="149" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="140"/>
+      <c r="F1" s="140"/>
+      <c r="G1" s="140"/>
+      <c r="H1" s="140"/>
+    </row>
+    <row r="2" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="115"/>
       <c r="C2" s="116"/>
       <c r="D2" s="115"/>
@@ -4045,7 +4569,7 @@
       <c r="F2" s="115"/>
       <c r="H2" s="115"/>
     </row>
-    <row r="3" spans="2:8" ht="12.75" customHeight="1">
+    <row r="3" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="115"/>
       <c r="C3" s="116"/>
       <c r="D3" s="115"/>
@@ -4053,19 +4577,19 @@
       <c r="F3" s="115"/>
       <c r="H3" s="115"/>
     </row>
-    <row r="4" spans="2:8" ht="12.75" customHeight="1">
+    <row r="4" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="56" t="s">
-        <v>164</v>
+        <v>149</v>
       </c>
       <c r="C4" s="116"/>
       <c r="D4" s="56" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="E4" s="115"/>
       <c r="F4" s="115"/>
       <c r="H4" s="115"/>
     </row>
-    <row r="5" spans="2:8" ht="13.15">
+    <row r="5" spans="2:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B5" s="115"/>
       <c r="C5" s="116"/>
       <c r="D5" s="117"/>
@@ -4074,7 +4598,7 @@
       <c r="G5" s="117"/>
       <c r="H5" s="117"/>
     </row>
-    <row r="6" spans="2:8" ht="12.75" customHeight="1">
+    <row r="6" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="115"/>
       <c r="C6" s="116"/>
       <c r="D6" s="115"/>
@@ -4082,38 +4606,38 @@
       <c r="F6" s="115"/>
       <c r="H6" s="115"/>
     </row>
-    <row r="7" spans="2:8" ht="12.75" customHeight="1">
+    <row r="7" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="113" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
       <c r="C7" s="116"/>
       <c r="D7" s="118" t="s">
-        <v>167</v>
+        <v>152</v>
       </c>
       <c r="E7" s="119" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="F7" s="119" t="s">
-        <v>169</v>
+        <v>154</v>
       </c>
       <c r="G7" s="119" t="s">
-        <v>170</v>
+        <v>155</v>
       </c>
       <c r="H7" s="120" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="13.5" customHeight="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C8" s="116"/>
       <c r="D8" s="121" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="E8" s="122"/>
       <c r="F8" s="122"/>
       <c r="G8" s="122"/>
       <c r="H8" s="123"/>
     </row>
-    <row r="9" spans="2:8" ht="14.25" customHeight="1">
+    <row r="9" spans="2:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="115"/>
       <c r="C9" s="124"/>
       <c r="D9" s="125"/>
@@ -4122,9 +4646,9 @@
       <c r="G9" s="126"/>
       <c r="H9" s="127"/>
     </row>
-    <row r="10" spans="2:8" ht="12.75" customHeight="1">
+    <row r="10" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="113" t="s">
-        <v>173</v>
+        <v>158</v>
       </c>
       <c r="C10" s="116"/>
       <c r="D10" s="128"/>
@@ -4133,9 +4657,9 @@
       <c r="G10" s="129"/>
       <c r="H10" s="130"/>
     </row>
-    <row r="11" spans="2:8" ht="12.75" customHeight="1">
+    <row r="11" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="56" t="s">
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="C11" s="116"/>
       <c r="D11" s="128"/>
@@ -4163,7 +4687,7 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
@@ -4179,10 +4703,10 @@
     <col min="14" max="23" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="21.75" customHeight="1">
+    <row r="2" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="70"/>
       <c r="C2" s="71" t="s">
-        <v>175</v>
+        <v>160</v>
       </c>
       <c r="D2" s="71"/>
       <c r="E2" s="71"/>
@@ -4195,20 +4719,20 @@
       <c r="L2" s="114"/>
       <c r="M2" s="114"/>
     </row>
-    <row r="3" spans="2:13" ht="21.75" customHeight="1">
+    <row r="3" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="70"/>
       <c r="D3" s="71"/>
       <c r="E3" s="71"/>
       <c r="F3" s="71"/>
       <c r="G3" s="71"/>
-      <c r="H3" s="145"/>
-      <c r="I3" s="135"/>
-      <c r="J3" s="135"/>
-      <c r="K3" s="135"/>
-      <c r="L3" s="135"/>
-      <c r="M3" s="135"/>
-    </row>
-    <row r="4" spans="2:13" ht="21.75" customHeight="1">
+      <c r="H3" s="151"/>
+      <c r="I3" s="140"/>
+      <c r="J3" s="140"/>
+      <c r="K3" s="140"/>
+      <c r="L3" s="140"/>
+      <c r="M3" s="140"/>
+    </row>
+    <row r="4" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="102"/>
       <c r="H4" s="102"/>
       <c r="I4" s="102"/>
@@ -4217,14 +4741,14 @@
       <c r="L4" s="102"/>
       <c r="M4" s="102"/>
     </row>
-    <row r="5" spans="2:13" ht="21.75" customHeight="1">
+    <row r="5" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="72" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="73"/>
       <c r="D5" s="74"/>
       <c r="E5" s="72" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="F5" s="73"/>
       <c r="G5" s="73"/>
@@ -4235,7 +4759,7 @@
       <c r="L5" s="73"/>
       <c r="M5" s="74"/>
     </row>
-    <row r="6" spans="2:13" ht="21.75" customHeight="1">
+    <row r="6" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="102"/>
       <c r="C6" s="102"/>
       <c r="D6" s="102"/>
@@ -4249,9 +4773,9 @@
       <c r="L6" s="102"/>
       <c r="M6" s="102"/>
     </row>
-    <row r="7" spans="2:13" ht="21.75" customHeight="1">
+    <row r="7" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="75" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="C7" s="102"/>
       <c r="D7" s="76"/>
@@ -4264,41 +4788,41 @@
       <c r="L7" s="102"/>
       <c r="M7" s="102"/>
     </row>
-    <row r="8" spans="2:13" ht="21.75" customHeight="1">
+    <row r="8" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="77" t="s">
-        <v>178</v>
+        <v>163</v>
       </c>
       <c r="C8" s="78" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
       <c r="D8" s="79" t="s">
-        <v>180</v>
+        <v>165</v>
       </c>
       <c r="E8" s="80" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="F8" s="81"/>
       <c r="G8" s="82"/>
       <c r="H8" s="83" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="I8" s="81"/>
       <c r="J8" s="82"/>
       <c r="K8" s="83" t="s">
-        <v>181</v>
+        <v>166</v>
       </c>
       <c r="L8" s="81"/>
       <c r="M8" s="82"/>
     </row>
-    <row r="9" spans="2:13" ht="9.75" customHeight="1">
+    <row r="9" spans="2:13" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="84" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="C9" s="85" t="s">
-        <v>183</v>
+        <v>168</v>
       </c>
       <c r="D9" s="86" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E9" s="87"/>
       <c r="F9" s="87"/>
@@ -4310,15 +4834,15 @@
       <c r="L9" s="87"/>
       <c r="M9" s="88"/>
     </row>
-    <row r="10" spans="2:13" ht="15" customHeight="1">
+    <row r="10" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="84" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="C10" s="131" t="s">
-        <v>186</v>
+        <v>171</v>
       </c>
       <c r="D10" s="86" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="E10" s="87"/>
       <c r="F10" s="87"/>
@@ -4330,39 +4854,39 @@
       <c r="L10" s="87"/>
       <c r="M10" s="88"/>
     </row>
-    <row r="11" spans="2:13" ht="15" customHeight="1">
+    <row r="11" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="90"/>
       <c r="C11" s="91"/>
       <c r="D11" s="69"/>
       <c r="E11" s="92" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="F11" s="92" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="G11" s="93" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="H11" s="94" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="I11" s="92" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="J11" s="93" t="s">
-        <v>190</v>
+        <v>175</v>
       </c>
       <c r="K11" s="94" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
       <c r="L11" s="92" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="M11" s="93" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13" ht="20.25" customHeight="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="95"/>
       <c r="C12" s="96"/>
       <c r="D12" s="97"/>
@@ -4376,9 +4900,9 @@
       <c r="L12" s="102"/>
       <c r="M12" s="99"/>
     </row>
-    <row r="13" spans="2:13" ht="20.25" customHeight="1">
+    <row r="13" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="105" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="C13" s="102"/>
       <c r="D13" s="106"/>
@@ -4392,12 +4916,12 @@
       <c r="L13" s="102"/>
       <c r="M13" s="99"/>
     </row>
-    <row r="14" spans="2:13" ht="20.25" customHeight="1">
+    <row r="14" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="101" t="s">
-        <v>162</v>
+        <v>147</v>
       </c>
       <c r="C14" s="102" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="D14" s="106"/>
       <c r="E14" s="103">
@@ -4414,10 +4938,10 @@
       <c r="L14" s="102"/>
       <c r="M14" s="99"/>
     </row>
-    <row r="15" spans="2:13" ht="20.25" customHeight="1">
+    <row r="15" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="105"/>
       <c r="C15" s="102" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
       <c r="D15" s="106"/>
       <c r="E15" s="103">
@@ -4425,7 +4949,7 @@
       </c>
       <c r="F15" s="102"/>
       <c r="G15" s="99" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
       <c r="H15" s="102"/>
       <c r="I15" s="102"/>
@@ -4434,10 +4958,10 @@
       <c r="L15" s="102"/>
       <c r="M15" s="99"/>
     </row>
-    <row r="16" spans="2:13" ht="20.25" customHeight="1">
+    <row r="16" spans="2:13" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="105"/>
       <c r="C16" s="102" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
       <c r="D16" s="106"/>
       <c r="E16" s="103">
@@ -4452,19 +4976,19 @@
       <c r="L16" s="102"/>
       <c r="M16" s="99"/>
     </row>
-    <row r="20" spans="3:3" ht="20.25" customHeight="1">
+    <row r="20" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C20" s="107" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" ht="20.25" customHeight="1">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C21" s="107" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" ht="20.25" customHeight="1">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="107" t="s">
-        <v>197</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -4481,21 +5005,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003344BE67D7EB984A84C06E190413FBFD" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9bce8fe95ceaf62c75926160740d41e2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9de94308-2297-4d04-a77d-26fce9df9395" xmlns:ns4="22375818-dcd7-42e4-9660-6b33e030de66" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1d88e73fd87162f28f317e92bcb9f946" ns3:_="" ns4:_="">
     <xsd:import namespace="9de94308-2297-4d04-a77d-26fce9df9395"/>
@@ -4672,14 +5181,53 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B130DE0C-7A28-4B03-98EC-F451E5EF5DFD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E8D0FC-D0F3-4D81-9707-E82360EDBF19}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9de94308-2297-4d04-a77d-26fce9df9395"/>
+    <ds:schemaRef ds:uri="22375818-dcd7-42e4-9660-6b33e030de66"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8039DF66-AB83-49D2-BABD-681C7E045BB6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B130DE0C-7A28-4B03-98EC-F451E5EF5DFD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8E8D0FC-D0F3-4D81-9707-E82360EDBF19}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8039DF66-AB83-49D2-BABD-681C7E045BB6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
avancer sur le excel
</commit_message>
<xml_diff>
--- a/Gestion_A_jmd.xlsx
+++ b/Gestion_A_jmd.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dilio\OneDrive\Bureau\ProjetDaleks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F77A27-B6D9-43B1-BED3-16D965CC7C18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745BF8D5-3E86-44F5-9CD9-AAD9AAA3DBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Méthodes SCRUM" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="290">
   <si>
     <t>Chiffrier de documentation de projets</t>
   </si>
@@ -811,9 +811,6 @@
     <t>while choix = choix_existant</t>
   </si>
   <si>
-    <t>facile,moyen,difficil</t>
-  </si>
-  <si>
     <t>affiche les differents niveau</t>
   </si>
   <si>
@@ -841,15 +838,6 @@
     <t>verifier collision</t>
   </si>
   <si>
-    <t>collision daleks docteur</t>
-  </si>
-  <si>
-    <t>collision daleks daleks</t>
-  </si>
-  <si>
-    <t>collision daleks ferraile</t>
-  </si>
-  <si>
     <t>if position_dacleks = postion_docteur si vrai fin de partie(perdu)</t>
   </si>
   <si>
@@ -922,9 +910,6 @@
     <t>press choix score</t>
   </si>
   <si>
-    <t>while choix = choix_existant =t</t>
-  </si>
-  <si>
     <t>while choix = choix_existant = z and if zapper &gt; 0</t>
   </si>
   <si>
@@ -961,9 +946,6 @@
     <t>plateau et toutes les entité qui le compose (docteur position defini au prealable ou aleatoire) (daleks placer aleatoirement0</t>
   </si>
   <si>
-    <t>et if  nb_daleks =0 fin de partie</t>
-  </si>
-  <si>
     <t>quitter le programe</t>
   </si>
   <si>
@@ -1058,6 +1040,75 @@
   </si>
   <si>
     <t>username, point</t>
+  </si>
+  <si>
+    <t>Airdejeu</t>
+  </si>
+  <si>
+    <t>Feraille</t>
+  </si>
+  <si>
+    <t>if collision daleks docteur</t>
+  </si>
+  <si>
+    <t>if collision daleks daleks</t>
+  </si>
+  <si>
+    <t>if collision daleks ferraile</t>
+  </si>
+  <si>
+    <t>print("facile - moyen - difficile")</t>
+  </si>
+  <si>
+    <t>if collision daleks et docteur = feraille</t>
+  </si>
+  <si>
+    <t>if  nb_daleks = 0 fin de partie, nb_zappeur += 1</t>
+  </si>
+  <si>
+    <t>fin_de_partie</t>
+  </si>
+  <si>
+    <t>while choix = choix_existant = t</t>
+  </si>
+  <si>
+    <t>Creer un fichier CSV</t>
+  </si>
+  <si>
+    <t>mouvement_permis</t>
+  </si>
+  <si>
+    <t>Haute</t>
+  </si>
+  <si>
+    <t>Nos fonctions</t>
+  </si>
+  <si>
+    <t>choix_possible</t>
+  </si>
+  <si>
+    <t>contact_dalek_docteur</t>
+  </si>
+  <si>
+    <t>contact_dalek_dalek</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>1h &lt;</t>
+  </si>
+  <si>
+    <t>1h</t>
+  </si>
+  <si>
+    <t>score_joueur</t>
+  </si>
+  <si>
+    <t>moyenne</t>
+  </si>
+  <si>
+    <t>2h</t>
   </si>
 </sst>
 </file>
@@ -1069,7 +1120,7 @@
     <numFmt numFmtId="165" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="166" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1171,8 +1222,27 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1190,8 +1260,62 @@
         <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFD9797"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="52">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -1790,12 +1914,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="51" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="156">
+  <cellXfs count="186">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2039,18 +2200,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2061,18 +2213,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="51" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="51" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="51" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="51" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="51" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="51" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2111,6 +2252,132 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="51" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="11" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="12" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2135,6 +2402,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFD9797"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2805,22 +3077,22 @@
       </c>
     </row>
     <row r="36" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F36" s="143"/>
-      <c r="G36" s="144"/>
-      <c r="H36" s="144"/>
-      <c r="I36" s="144"/>
+      <c r="F36" s="129"/>
+      <c r="G36" s="130"/>
+      <c r="H36" s="130"/>
+      <c r="I36" s="130"/>
     </row>
     <row r="37" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F37" s="144"/>
-      <c r="G37" s="144"/>
-      <c r="H37" s="144"/>
-      <c r="I37" s="144"/>
+      <c r="F37" s="130"/>
+      <c r="G37" s="130"/>
+      <c r="H37" s="130"/>
+      <c r="I37" s="130"/>
     </row>
     <row r="38" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F38" s="144"/>
-      <c r="G38" s="144"/>
-      <c r="H38" s="144"/>
-      <c r="I38" s="144"/>
+      <c r="F38" s="130"/>
+      <c r="G38" s="130"/>
+      <c r="H38" s="130"/>
+      <c r="I38" s="130"/>
     </row>
     <row r="39" spans="6:9" ht="17.25" customHeight="1">
       <c r="F39" s="112"/>
@@ -2829,22 +3101,22 @@
       <c r="I39" s="112"/>
     </row>
     <row r="40" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F40" s="143"/>
-      <c r="G40" s="144"/>
-      <c r="H40" s="144"/>
-      <c r="I40" s="144"/>
+      <c r="F40" s="129"/>
+      <c r="G40" s="130"/>
+      <c r="H40" s="130"/>
+      <c r="I40" s="130"/>
     </row>
     <row r="41" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F41" s="144"/>
-      <c r="G41" s="144"/>
-      <c r="H41" s="144"/>
-      <c r="I41" s="144"/>
+      <c r="F41" s="130"/>
+      <c r="G41" s="130"/>
+      <c r="H41" s="130"/>
+      <c r="I41" s="130"/>
     </row>
     <row r="42" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F42" s="144"/>
-      <c r="G42" s="144"/>
-      <c r="H42" s="144"/>
-      <c r="I42" s="144"/>
+      <c r="F42" s="130"/>
+      <c r="G42" s="130"/>
+      <c r="H42" s="130"/>
+      <c r="I42" s="130"/>
     </row>
     <row r="43" spans="6:9" ht="17.25" customHeight="1">
       <c r="F43" s="112"/>
@@ -2859,34 +3131,34 @@
       <c r="I44" s="112"/>
     </row>
     <row r="45" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F45" s="143"/>
-      <c r="G45" s="144"/>
-      <c r="H45" s="144"/>
-      <c r="I45" s="144"/>
+      <c r="F45" s="129"/>
+      <c r="G45" s="130"/>
+      <c r="H45" s="130"/>
+      <c r="I45" s="130"/>
     </row>
     <row r="46" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F46" s="144"/>
-      <c r="G46" s="144"/>
-      <c r="H46" s="144"/>
-      <c r="I46" s="144"/>
+      <c r="F46" s="130"/>
+      <c r="G46" s="130"/>
+      <c r="H46" s="130"/>
+      <c r="I46" s="130"/>
     </row>
     <row r="47" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F47" s="144"/>
-      <c r="G47" s="144"/>
-      <c r="H47" s="144"/>
-      <c r="I47" s="144"/>
+      <c r="F47" s="130"/>
+      <c r="G47" s="130"/>
+      <c r="H47" s="130"/>
+      <c r="I47" s="130"/>
     </row>
     <row r="48" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F48" s="144"/>
-      <c r="G48" s="144"/>
-      <c r="H48" s="144"/>
-      <c r="I48" s="144"/>
+      <c r="F48" s="130"/>
+      <c r="G48" s="130"/>
+      <c r="H48" s="130"/>
+      <c r="I48" s="130"/>
     </row>
     <row r="49" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F49" s="144"/>
-      <c r="G49" s="144"/>
-      <c r="H49" s="144"/>
-      <c r="I49" s="144"/>
+      <c r="F49" s="130"/>
+      <c r="G49" s="130"/>
+      <c r="H49" s="130"/>
+      <c r="I49" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2906,7 +3178,7 @@
   <dimension ref="B2:E46"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="66" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3008,7 +3280,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B13" s="145" t="s">
+      <c r="B13" s="131" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -3022,19 +3294,19 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B14" s="146"/>
+      <c r="B14" s="132"/>
       <c r="C14" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="D14" s="134" t="s">
-        <v>214</v>
+      <c r="D14" s="125" t="s">
+        <v>210</v>
       </c>
       <c r="E14" s="41" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="15" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B15" s="146"/>
+      <c r="B15" s="132"/>
       <c r="C15" s="22" t="s">
         <v>65</v>
       </c>
@@ -3046,19 +3318,19 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B16" s="146"/>
-      <c r="C16" s="135" t="s">
-        <v>215</v>
-      </c>
-      <c r="D16" s="134" t="s">
-        <v>260</v>
+      <c r="B16" s="132"/>
+      <c r="C16" s="126" t="s">
+        <v>211</v>
+      </c>
+      <c r="D16" s="125" t="s">
+        <v>254</v>
       </c>
       <c r="E16" s="41" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B17" s="146"/>
+      <c r="B17" s="132"/>
       <c r="C17" s="22" t="s">
         <v>67</v>
       </c>
@@ -3070,7 +3342,7 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B18" s="146"/>
+      <c r="B18" s="132"/>
       <c r="C18" s="22" t="s">
         <v>182</v>
       </c>
@@ -3080,7 +3352,7 @@
       <c r="E18" s="41"/>
     </row>
     <row r="19" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B19" s="146"/>
+      <c r="B19" s="132"/>
       <c r="C19" s="22" t="s">
         <v>69</v>
       </c>
@@ -3088,107 +3360,107 @@
         <v>70</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B20" s="146"/>
+      <c r="B20" s="132"/>
       <c r="C20" s="22" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B21" s="146"/>
+      <c r="B21" s="132"/>
       <c r="C21" s="22" t="s">
         <v>91</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
     </row>
     <row r="22" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B22" s="146"/>
+      <c r="B22" s="132"/>
       <c r="C22" s="22" t="s">
         <v>71</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>268</v>
-      </c>
-      <c r="E22" s="133" t="s">
-        <v>211</v>
+        <v>262</v>
+      </c>
+      <c r="E22" s="124" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B23" s="146"/>
+      <c r="B23" s="132"/>
       <c r="C23" s="22" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>265</v>
-      </c>
-      <c r="E23" s="133" t="s">
         <v>259</v>
       </c>
+      <c r="E23" s="124" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="24" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B24" s="146"/>
+      <c r="B24" s="132"/>
       <c r="C24" s="22" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>266</v>
-      </c>
-      <c r="E24" s="133" t="s">
-        <v>259</v>
+        <v>260</v>
+      </c>
+      <c r="E24" s="124" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B25" s="146"/>
+      <c r="B25" s="132"/>
       <c r="C25" s="22" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>267</v>
-      </c>
-      <c r="E25" s="133" t="s">
-        <v>259</v>
+        <v>261</v>
+      </c>
+      <c r="E25" s="124" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B26" s="147"/>
+      <c r="B26" s="133"/>
       <c r="C26" s="19" t="s">
         <v>73</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>269</v>
-      </c>
-      <c r="E26" s="132" t="s">
-        <v>210</v>
+        <v>263</v>
+      </c>
+      <c r="E26" s="123" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="27" spans="2:5" ht="12.75" customHeight="1">
       <c r="B27" s="108"/>
       <c r="C27" s="22" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>271</v>
-      </c>
-      <c r="E27" s="133" t="s">
-        <v>272</v>
+        <v>265</v>
+      </c>
+      <c r="E27" s="124" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B28" s="145" t="s">
+      <c r="B28" s="131" t="s">
         <v>75</v>
       </c>
       <c r="C28" s="23" t="s">
@@ -3202,135 +3474,135 @@
       </c>
     </row>
     <row r="29" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B29" s="146"/>
+      <c r="B29" s="132"/>
       <c r="C29" s="22" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E29" s="41" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
     </row>
     <row r="30" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B30" s="146"/>
+      <c r="B30" s="132"/>
       <c r="C30" s="22" t="s">
         <v>61</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="E30" s="41" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B31" s="146"/>
+      <c r="B31" s="132"/>
       <c r="C31" s="22" t="s">
         <v>71</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B32" s="146"/>
+      <c r="B32" s="132"/>
       <c r="C32" s="22"/>
       <c r="D32" s="18"/>
       <c r="E32" s="41"/>
     </row>
     <row r="33" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B33" s="146"/>
+      <c r="B33" s="132"/>
       <c r="C33" s="22"/>
       <c r="D33" s="18"/>
       <c r="E33" s="41"/>
     </row>
     <row r="34" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B34" s="146"/>
+      <c r="B34" s="132"/>
       <c r="C34" s="22"/>
       <c r="D34" s="18"/>
       <c r="E34" s="41"/>
     </row>
     <row r="35" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B35" s="146"/>
+      <c r="B35" s="132"/>
       <c r="C35" s="22"/>
       <c r="D35" s="18"/>
       <c r="E35" s="41"/>
     </row>
     <row r="36" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B36" s="147"/>
+      <c r="B36" s="133"/>
       <c r="C36" s="19"/>
       <c r="D36" s="40"/>
       <c r="E36" s="20"/>
     </row>
     <row r="37" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B37" s="145" t="s">
+      <c r="B37" s="131" t="s">
         <v>76</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="D37" s="39" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="E37" s="21" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
     </row>
     <row r="38" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B38" s="146"/>
+      <c r="B38" s="132"/>
       <c r="C38" s="22"/>
       <c r="D38" s="18"/>
       <c r="E38" s="41"/>
     </row>
     <row r="39" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B39" s="146"/>
+      <c r="B39" s="132"/>
       <c r="C39" s="22"/>
       <c r="D39" s="18"/>
       <c r="E39" s="41"/>
     </row>
     <row r="40" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B40" s="146"/>
+      <c r="B40" s="132"/>
       <c r="C40" s="22"/>
       <c r="D40" s="18"/>
       <c r="E40" s="41"/>
     </row>
     <row r="41" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B41" s="146"/>
+      <c r="B41" s="132"/>
       <c r="C41" s="22"/>
       <c r="D41" s="18"/>
       <c r="E41" s="41"/>
     </row>
     <row r="42" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B42" s="146"/>
+      <c r="B42" s="132"/>
       <c r="C42" s="22"/>
       <c r="D42" s="18"/>
       <c r="E42" s="41"/>
     </row>
     <row r="43" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B43" s="146"/>
+      <c r="B43" s="132"/>
       <c r="C43" s="22"/>
       <c r="D43" s="18"/>
       <c r="E43" s="41"/>
     </row>
     <row r="44" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B44" s="146"/>
+      <c r="B44" s="132"/>
       <c r="C44" s="22"/>
       <c r="D44" s="18"/>
       <c r="E44" s="41"/>
     </row>
     <row r="45" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B45" s="146"/>
+      <c r="B45" s="132"/>
       <c r="C45" s="22"/>
       <c r="D45" s="18"/>
       <c r="E45" s="41"/>
     </row>
     <row r="46" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B46" s="147"/>
+      <c r="B46" s="133"/>
       <c r="C46" s="24"/>
       <c r="D46" s="25"/>
       <c r="E46" s="46"/>
@@ -3350,10 +3622,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:F105"/>
+  <dimension ref="B2:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" zoomScale="73" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView topLeftCell="F9" zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1"/>
@@ -3378,20 +3650,20 @@
     </row>
     <row r="3" spans="2:6" ht="89.4" customHeight="1">
       <c r="B3" s="109"/>
-      <c r="C3" s="148" t="s">
+      <c r="C3" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
+      <c r="D3" s="130"/>
+      <c r="E3" s="130"/>
       <c r="F3" s="109"/>
     </row>
     <row r="4" spans="2:6" ht="30.75" customHeight="1">
       <c r="B4" s="110"/>
-      <c r="C4" s="149" t="s">
+      <c r="C4" s="135" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="144"/>
-      <c r="E4" s="144"/>
+      <c r="D4" s="130"/>
+      <c r="E4" s="130"/>
       <c r="F4" s="110"/>
     </row>
     <row r="5" spans="2:6" ht="21" customHeight="1">
@@ -3471,636 +3743,654 @@
       <c r="D12" s="32"/>
     </row>
     <row r="13" spans="2:6" ht="18" customHeight="1">
-      <c r="B13" s="136" t="s">
+      <c r="B13" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="137" t="s">
+      <c r="C13" s="159" t="s">
         <v>187</v>
       </c>
-      <c r="D13" s="138" t="s">
+      <c r="D13" s="143" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="136"/>
-      <c r="F13" s="136"/>
+      <c r="E13" s="142"/>
+      <c r="F13" s="142"/>
     </row>
     <row r="14" spans="2:6" ht="18" customHeight="1">
-      <c r="B14" s="139"/>
-      <c r="C14" s="140"/>
-      <c r="D14" s="139"/>
-      <c r="E14" s="141" t="s">
+      <c r="B14" s="144"/>
+      <c r="C14" s="145"/>
+      <c r="D14" s="144"/>
+      <c r="E14" s="146" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="136"/>
+      <c r="F14" s="142"/>
     </row>
     <row r="15" spans="2:6" ht="18" customHeight="1">
-      <c r="B15" s="139"/>
-      <c r="C15" s="142"/>
-      <c r="D15" s="139"/>
-      <c r="E15" s="141" t="s">
+      <c r="B15" s="144"/>
+      <c r="C15" s="147"/>
+      <c r="D15" s="144"/>
+      <c r="E15" s="146" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="141"/>
+      <c r="F15" s="146"/>
     </row>
     <row r="16" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B16" s="136"/>
-      <c r="C16" s="136"/>
-      <c r="D16" s="136"/>
-      <c r="E16" s="141" t="s">
+      <c r="B16" s="142"/>
+      <c r="C16" s="142"/>
+      <c r="D16" s="142"/>
+      <c r="E16" s="146" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="136"/>
+      <c r="F16" s="142"/>
     </row>
     <row r="17" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B17" s="136"/>
-      <c r="C17" s="136"/>
-      <c r="D17" s="141"/>
-      <c r="E17" s="136" t="s">
+      <c r="B17" s="142"/>
+      <c r="C17" s="142"/>
+      <c r="D17" s="146"/>
+      <c r="E17" s="142" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="136"/>
+      <c r="F17" s="142"/>
     </row>
     <row r="18" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B18" s="136"/>
-      <c r="C18" s="136"/>
-      <c r="D18" s="136"/>
-      <c r="E18" s="141" t="s">
+      <c r="B18" s="142"/>
+      <c r="C18" s="142"/>
+      <c r="D18" s="142"/>
+      <c r="E18" s="146" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="141" t="s">
+      <c r="F18" s="146" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="19" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B19" s="136"/>
-      <c r="C19" s="141" t="s">
+      <c r="B19" s="127" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="160" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="141" t="s">
+      <c r="D19" s="128" t="s">
         <v>188</v>
       </c>
-      <c r="E19" s="136"/>
-      <c r="F19" s="141" t="s">
+      <c r="E19" s="127"/>
+      <c r="F19" s="128" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="20" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B20" s="136"/>
-      <c r="C20" s="136"/>
-      <c r="D20" s="141"/>
-      <c r="E20" s="141" t="s">
+      <c r="B20" s="127"/>
+      <c r="C20" s="127"/>
+      <c r="D20" s="128"/>
+      <c r="E20" s="128" t="s">
         <v>99</v>
       </c>
-      <c r="F20" s="141"/>
+      <c r="F20" s="128"/>
     </row>
     <row r="21" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B21" s="136"/>
-      <c r="C21" s="136"/>
-      <c r="D21" s="141"/>
-      <c r="E21" s="141" t="s">
+      <c r="B21" s="127"/>
+      <c r="C21" s="127"/>
+      <c r="D21" s="128"/>
+      <c r="E21" s="128" t="s">
+        <v>227</v>
+      </c>
+      <c r="F21" s="128"/>
+    </row>
+    <row r="22" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B22" s="127"/>
+      <c r="C22" s="127"/>
+      <c r="D22" s="128" t="s">
+        <v>228</v>
+      </c>
+      <c r="E22" s="128"/>
+      <c r="F22" s="128"/>
+    </row>
+    <row r="23" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B23" s="127"/>
+      <c r="C23" s="127"/>
+      <c r="D23" s="128"/>
+      <c r="E23" s="128" t="s">
+        <v>277</v>
+      </c>
+      <c r="F23" s="128"/>
+    </row>
+    <row r="24" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B24" s="128" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="127"/>
+      <c r="D24" s="128"/>
+      <c r="E24" s="128" t="s">
+        <v>190</v>
+      </c>
+      <c r="F24" s="128" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B25" s="128" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25" s="127"/>
+      <c r="D25" s="128" t="s">
+        <v>191</v>
+      </c>
+      <c r="E25" s="128"/>
+      <c r="F25" s="128"/>
+    </row>
+    <row r="26" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B26" s="127"/>
+      <c r="C26" s="127"/>
+      <c r="D26" s="128"/>
+      <c r="E26" s="128" t="s">
+        <v>192</v>
+      </c>
+      <c r="F26" s="128" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" ht="15" customHeight="1">
+      <c r="B27" s="127"/>
+      <c r="C27" s="127"/>
+      <c r="D27" s="127"/>
+      <c r="E27" s="128" t="s">
+        <v>101</v>
+      </c>
+      <c r="F27" s="128" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B28" s="127"/>
+      <c r="C28" s="127"/>
+      <c r="D28" s="127"/>
+      <c r="E28" s="128" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="128" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B29" s="127"/>
+      <c r="C29" s="127"/>
+      <c r="D29" s="127"/>
+      <c r="E29" s="128" t="s">
+        <v>103</v>
+      </c>
+      <c r="F29" s="128" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B30" s="148" t="s">
+        <v>91</v>
+      </c>
+      <c r="C30" s="161" t="s">
+        <v>104</v>
+      </c>
+      <c r="D30" s="148"/>
+      <c r="E30" s="148"/>
+      <c r="F30" s="149" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B31" s="148"/>
+      <c r="C31" s="148"/>
+      <c r="D31" s="149"/>
+      <c r="E31" s="149" t="s">
+        <v>194</v>
+      </c>
+      <c r="F31" s="149" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B32" s="148"/>
+      <c r="C32" s="148"/>
+      <c r="D32" s="149"/>
+      <c r="E32" s="148" t="s">
+        <v>107</v>
+      </c>
+      <c r="F32" s="149"/>
+    </row>
+    <row r="33" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B33" s="148"/>
+      <c r="C33" s="148"/>
+      <c r="D33" s="149"/>
+      <c r="E33" s="149" t="s">
+        <v>195</v>
+      </c>
+      <c r="F33" s="149" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B34" s="148" t="s">
+        <v>89</v>
+      </c>
+      <c r="C34" s="161" t="s">
+        <v>198</v>
+      </c>
+      <c r="D34" s="148"/>
+      <c r="E34" s="149" t="s">
+        <v>269</v>
+      </c>
+      <c r="F34" s="149" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B35" s="148"/>
+      <c r="C35" s="148"/>
+      <c r="D35" s="148"/>
+      <c r="E35" s="149" t="s">
+        <v>270</v>
+      </c>
+      <c r="F35" s="149" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B36" s="148"/>
+      <c r="C36" s="148"/>
+      <c r="D36" s="148"/>
+      <c r="E36" s="149" t="s">
+        <v>271</v>
+      </c>
+      <c r="F36" s="149" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B37" s="148"/>
+      <c r="C37" s="148"/>
+      <c r="D37" s="148"/>
+      <c r="E37" s="149" t="s">
+        <v>231</v>
+      </c>
+      <c r="F37" s="149" t="s">
         <v>232</v>
       </c>
-      <c r="F21" s="141"/>
-    </row>
-    <row r="22" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B22" s="136"/>
-      <c r="C22" s="136"/>
-      <c r="D22" s="141" t="s">
-        <v>233</v>
-      </c>
-      <c r="E22" s="141"/>
-      <c r="F22" s="141"/>
-    </row>
-    <row r="23" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B23" s="136"/>
-      <c r="C23" s="136"/>
-      <c r="D23" s="141"/>
-      <c r="E23" s="141" t="s">
-        <v>191</v>
-      </c>
-      <c r="F23" s="141" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B24" s="136"/>
-      <c r="C24" s="136"/>
-      <c r="D24" s="141" t="s">
-        <v>192</v>
-      </c>
-      <c r="E24" s="141"/>
-      <c r="F24" s="141"/>
-    </row>
-    <row r="25" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B25" s="136"/>
-      <c r="C25" s="136"/>
-      <c r="D25" s="141"/>
-      <c r="E25" s="141" t="s">
-        <v>193</v>
-      </c>
-      <c r="F25" s="141" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" ht="15" customHeight="1">
-      <c r="B26" s="136"/>
-      <c r="C26" s="136"/>
-      <c r="D26" s="136"/>
-      <c r="E26" s="141" t="s">
-        <v>101</v>
-      </c>
-      <c r="F26" s="141" t="s">
+    </row>
+    <row r="38" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B38" s="148"/>
+      <c r="C38" s="148"/>
+      <c r="D38" s="148"/>
+      <c r="E38" s="149" t="s">
+        <v>229</v>
+      </c>
+      <c r="F38" s="149" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B39" s="148"/>
+      <c r="C39" s="148"/>
+      <c r="D39" s="148"/>
+      <c r="E39" s="149" t="s">
+        <v>102</v>
+      </c>
+      <c r="F39" s="149"/>
+    </row>
+    <row r="40" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B40" s="150" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="162" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="151" t="s">
+        <v>105</v>
+      </c>
+      <c r="E40" s="150"/>
+      <c r="F40" s="151" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B41" s="150"/>
+      <c r="C41" s="150"/>
+      <c r="D41" s="150"/>
+      <c r="E41" s="151" t="s">
+        <v>202</v>
+      </c>
+      <c r="F41" s="151" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B42" s="150"/>
+      <c r="C42" s="150"/>
+      <c r="D42" s="150"/>
+      <c r="E42" s="150" t="s">
+        <v>107</v>
+      </c>
+      <c r="F42" s="151"/>
+    </row>
+    <row r="43" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B43" s="150" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="162" t="s">
+        <v>204</v>
+      </c>
+      <c r="D43" s="150"/>
+      <c r="E43" s="151" t="s">
+        <v>269</v>
+      </c>
+      <c r="F43" s="151" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B44" s="150"/>
+      <c r="C44" s="151"/>
+      <c r="D44" s="150"/>
+      <c r="E44" s="151" t="s">
+        <v>270</v>
+      </c>
+      <c r="F44" s="151" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B45" s="150"/>
+      <c r="C45" s="151"/>
+      <c r="D45" s="150"/>
+      <c r="E45" s="151" t="s">
+        <v>271</v>
+      </c>
+      <c r="F45" s="151" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B46" s="150"/>
+      <c r="C46" s="151"/>
+      <c r="D46" s="150"/>
+      <c r="E46" s="151" t="s">
+        <v>273</v>
+      </c>
+      <c r="F46" s="150"/>
+    </row>
+    <row r="47" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B47" s="150"/>
+      <c r="C47" s="151"/>
+      <c r="D47" s="150"/>
+      <c r="E47" s="151" t="s">
+        <v>102</v>
+      </c>
+      <c r="F47" s="150"/>
+    </row>
+    <row r="48" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B48" s="152" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="163" t="s">
+        <v>205</v>
+      </c>
+      <c r="D48" s="153" t="s">
+        <v>105</v>
+      </c>
+      <c r="E48" s="152"/>
+      <c r="F48" s="153" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B49" s="152"/>
+      <c r="C49" s="152"/>
+      <c r="D49" s="152"/>
+      <c r="E49" s="153" t="s">
+        <v>208</v>
+      </c>
+      <c r="F49" s="153" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B50" s="152"/>
+      <c r="C50" s="152"/>
+      <c r="D50" s="152"/>
+      <c r="E50" s="153" t="s">
+        <v>231</v>
+      </c>
+      <c r="F50" s="153" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B51" s="152"/>
+      <c r="C51" s="152"/>
+      <c r="D51" s="152"/>
+      <c r="E51" s="153" t="s">
+        <v>195</v>
+      </c>
+      <c r="F51" s="153"/>
+    </row>
+    <row r="52" spans="2:6" ht="18" customHeight="1">
+      <c r="B52" s="152" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="163" t="s">
+        <v>198</v>
+      </c>
+      <c r="D52" s="154"/>
+      <c r="E52" s="153" t="s">
+        <v>269</v>
+      </c>
+      <c r="F52" s="153" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="18" customHeight="1">
+      <c r="B53" s="152"/>
+      <c r="C53" s="153"/>
+      <c r="D53" s="154"/>
+      <c r="E53" s="153" t="s">
+        <v>270</v>
+      </c>
+      <c r="F53" s="153" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" ht="18" customHeight="1">
+      <c r="B54" s="152"/>
+      <c r="C54" s="153"/>
+      <c r="D54" s="154"/>
+      <c r="E54" s="153" t="s">
+        <v>273</v>
+      </c>
+      <c r="F54" s="153" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" ht="18" customHeight="1">
+      <c r="B55" s="152"/>
+      <c r="C55" s="153"/>
+      <c r="D55" s="154"/>
+      <c r="E55" s="153" t="s">
+        <v>102</v>
+      </c>
+      <c r="F55" s="152"/>
+    </row>
+    <row r="56" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B56" s="155" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="164" t="s">
+        <v>213</v>
+      </c>
+      <c r="D56" s="155"/>
+      <c r="E56" s="156" t="s">
+        <v>212</v>
+      </c>
+      <c r="F56" s="156" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B57" s="155"/>
+      <c r="C57" s="156"/>
+      <c r="D57" s="155"/>
+      <c r="E57" s="156" t="s">
+        <v>215</v>
+      </c>
+      <c r="F57" s="156" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B58" s="155"/>
+      <c r="C58" s="155"/>
+      <c r="D58" s="155"/>
+      <c r="E58" s="156" t="s">
+        <v>218</v>
+      </c>
+      <c r="F58" s="156" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B59" s="155"/>
+      <c r="C59" s="155"/>
+      <c r="D59" s="156" t="s">
+        <v>219</v>
+      </c>
+      <c r="E59" s="155"/>
+      <c r="F59" s="156" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B60" s="155"/>
+      <c r="C60" s="155"/>
+      <c r="D60" s="155"/>
+      <c r="E60" s="156" t="s">
+        <v>95</v>
+      </c>
+      <c r="F60" s="155"/>
+    </row>
+    <row r="61" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B61" s="155"/>
+      <c r="C61" s="155"/>
+      <c r="D61" s="155"/>
+      <c r="E61" s="155" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" s="155"/>
+    </row>
+    <row r="62" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B62" s="155"/>
+      <c r="C62" s="155"/>
+      <c r="D62" s="155"/>
+      <c r="E62" s="156" t="s">
+        <v>97</v>
+      </c>
+      <c r="F62" s="156" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B63" s="157" t="s">
+        <v>89</v>
+      </c>
+      <c r="C63" s="165" t="s">
+        <v>221</v>
+      </c>
+      <c r="D63" s="158" t="s">
+        <v>222</v>
+      </c>
+      <c r="E63" s="157"/>
+      <c r="F63" s="158" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B64" s="157"/>
+      <c r="C64" s="157"/>
+      <c r="D64" s="157"/>
+      <c r="E64" s="158" t="s">
+        <v>225</v>
+      </c>
+      <c r="F64" s="157"/>
+    </row>
+    <row r="65" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B65" s="157"/>
+      <c r="C65" s="157"/>
+      <c r="D65" s="157"/>
+      <c r="E65" s="158" t="s">
+        <v>226</v>
+      </c>
+      <c r="F65" s="157"/>
+    </row>
+    <row r="66" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B66" s="157"/>
+      <c r="C66" s="157"/>
+      <c r="D66" s="158" t="s">
+        <v>219</v>
+      </c>
+      <c r="E66" s="157"/>
+      <c r="F66" s="158" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B67" s="157"/>
+      <c r="C67" s="157"/>
+      <c r="D67" s="157"/>
+      <c r="E67" s="158" t="s">
+        <v>97</v>
+      </c>
+      <c r="F67" s="158" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B68" s="157" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="165" t="s">
+        <v>235</v>
+      </c>
+      <c r="D68" s="158" t="s">
+        <v>237</v>
+      </c>
+      <c r="E68" s="157"/>
+      <c r="F68" s="158" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B69" s="157"/>
+      <c r="C69" s="157"/>
+      <c r="D69" s="157"/>
+      <c r="E69" s="158" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="27" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B27" s="136"/>
-      <c r="C27" s="136"/>
-      <c r="D27" s="136"/>
-      <c r="E27" s="141" t="s">
-        <v>102</v>
-      </c>
-      <c r="F27" s="141" t="s">
+      <c r="F69" s="157"/>
+    </row>
+    <row r="70" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B70" s="157"/>
+      <c r="C70" s="157"/>
+      <c r="D70" s="157"/>
+      <c r="E70" s="158" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="28" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B28" s="136"/>
-      <c r="C28" s="136"/>
-      <c r="D28" s="136"/>
-      <c r="E28" s="141" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="141" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B29" s="136"/>
-      <c r="C29" s="136" t="s">
-        <v>104</v>
-      </c>
-      <c r="D29" s="136"/>
-      <c r="E29" s="136"/>
-      <c r="F29" s="141" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B30" s="136"/>
-      <c r="C30" s="136"/>
-      <c r="D30" s="141"/>
-      <c r="E30" s="141" t="s">
-        <v>195</v>
-      </c>
-      <c r="F30" s="141" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B31" s="136"/>
-      <c r="C31" s="136"/>
-      <c r="D31" s="141"/>
-      <c r="E31" s="136" t="s">
-        <v>107</v>
-      </c>
-      <c r="F31" s="141"/>
-    </row>
-    <row r="32" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B32" s="136"/>
-      <c r="C32" s="136"/>
-      <c r="D32" s="141"/>
-      <c r="E32" s="141" t="s">
-        <v>196</v>
-      </c>
-      <c r="F32" s="141" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="33" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B33" s="136"/>
-      <c r="C33" s="141" t="s">
-        <v>199</v>
-      </c>
-      <c r="D33" s="136"/>
-      <c r="E33" s="141" t="s">
-        <v>200</v>
-      </c>
-      <c r="F33" s="141" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="34" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B34" s="136"/>
-      <c r="C34" s="136"/>
-      <c r="D34" s="136"/>
-      <c r="E34" s="141" t="s">
-        <v>201</v>
-      </c>
-      <c r="F34" s="141" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B35" s="136"/>
-      <c r="C35" s="136"/>
-      <c r="D35" s="136"/>
-      <c r="E35" s="141" t="s">
-        <v>202</v>
-      </c>
-      <c r="F35" s="141" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B36" s="136"/>
-      <c r="C36" s="136"/>
-      <c r="D36" s="136"/>
-      <c r="E36" s="141" t="s">
-        <v>236</v>
-      </c>
-      <c r="F36" s="141" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="37" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B37" s="136"/>
-      <c r="C37" s="136"/>
-      <c r="D37" s="136"/>
-      <c r="E37" s="141" t="s">
-        <v>234</v>
-      </c>
-      <c r="F37" s="141" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B38" s="136"/>
-      <c r="C38" s="136"/>
-      <c r="D38" s="136"/>
-      <c r="E38" s="141" t="s">
-        <v>102</v>
-      </c>
-      <c r="F38" s="141"/>
-    </row>
-    <row r="39" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B39" s="136"/>
-      <c r="C39" s="141" t="s">
-        <v>72</v>
-      </c>
-      <c r="D39" s="141" t="s">
-        <v>105</v>
-      </c>
-      <c r="E39" s="136"/>
-      <c r="F39" s="141" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B40" s="136"/>
-      <c r="C40" s="136"/>
-      <c r="D40" s="136"/>
-      <c r="E40" s="141" t="s">
-        <v>206</v>
-      </c>
-      <c r="F40" s="141" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="41" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B41" s="136"/>
-      <c r="C41" s="136"/>
-      <c r="D41" s="136"/>
-      <c r="E41" s="136" t="s">
-        <v>107</v>
-      </c>
-      <c r="F41" s="141"/>
-    </row>
-    <row r="42" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B42" s="136"/>
-      <c r="C42" s="141" t="s">
-        <v>208</v>
-      </c>
-      <c r="D42" s="136"/>
-      <c r="E42" s="141" t="s">
-        <v>200</v>
-      </c>
-      <c r="F42" s="136"/>
-    </row>
-    <row r="43" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B43" s="136"/>
-      <c r="C43" s="141"/>
-      <c r="D43" s="136"/>
-      <c r="E43" s="141" t="s">
-        <v>201</v>
-      </c>
-      <c r="F43" s="136"/>
-    </row>
-    <row r="44" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B44" s="136"/>
-      <c r="C44" s="141"/>
-      <c r="D44" s="136"/>
-      <c r="E44" s="141" t="s">
-        <v>202</v>
-      </c>
-      <c r="F44" s="136"/>
-    </row>
-    <row r="45" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B45" s="136"/>
-      <c r="C45" s="141"/>
-      <c r="D45" s="136"/>
-      <c r="E45" s="141" t="s">
-        <v>236</v>
-      </c>
-      <c r="F45" s="136"/>
-    </row>
-    <row r="46" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B46" s="136"/>
-      <c r="C46" s="141"/>
-      <c r="D46" s="136"/>
-      <c r="E46" s="141" t="s">
-        <v>234</v>
-      </c>
-      <c r="F46" s="136"/>
-    </row>
-    <row r="47" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B47" s="136"/>
-      <c r="C47" s="141"/>
-      <c r="D47" s="136"/>
-      <c r="E47" s="141" t="s">
-        <v>102</v>
-      </c>
-      <c r="F47" s="136"/>
-    </row>
-    <row r="48" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B48" s="136"/>
-      <c r="C48" s="141" t="s">
-        <v>209</v>
-      </c>
-      <c r="D48" s="141" t="s">
-        <v>105</v>
-      </c>
-      <c r="E48" s="136"/>
-      <c r="F48" s="141" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B49" s="136"/>
-      <c r="C49" s="136"/>
-      <c r="D49" s="136"/>
-      <c r="E49" s="141" t="s">
-        <v>212</v>
-      </c>
-      <c r="F49" s="141" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B50" s="136"/>
-      <c r="C50" s="136"/>
-      <c r="D50" s="136"/>
-      <c r="E50" s="141" t="s">
-        <v>236</v>
-      </c>
-      <c r="F50" s="141" t="s">
+      <c r="F70" s="157"/>
+    </row>
+    <row r="71" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B71" s="157"/>
+      <c r="C71" s="157"/>
+      <c r="D71" s="157"/>
+      <c r="E71" s="158" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="51" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B51" s="136"/>
-      <c r="C51" s="136"/>
-      <c r="D51" s="136"/>
-      <c r="E51" s="141" t="s">
-        <v>196</v>
-      </c>
-      <c r="F51" s="141"/>
-    </row>
-    <row r="52" spans="2:6" ht="18" customHeight="1">
-      <c r="B52" s="136"/>
-      <c r="C52" s="141" t="s">
-        <v>199</v>
-      </c>
-      <c r="D52" s="140"/>
-      <c r="E52" s="141" t="s">
-        <v>200</v>
-      </c>
-      <c r="F52" s="136"/>
-    </row>
-    <row r="53" spans="2:6" ht="18" customHeight="1">
-      <c r="B53" s="136"/>
-      <c r="C53" s="141"/>
-      <c r="D53" s="140"/>
-      <c r="E53" s="141" t="s">
-        <v>201</v>
-      </c>
-      <c r="F53" s="136"/>
-    </row>
-    <row r="54" spans="2:6" ht="18" customHeight="1">
-      <c r="B54" s="136"/>
-      <c r="C54" s="141"/>
-      <c r="D54" s="140"/>
-      <c r="E54" s="141" t="s">
-        <v>202</v>
-      </c>
-      <c r="F54" s="136"/>
-    </row>
-    <row r="55" spans="2:6" ht="18" customHeight="1">
-      <c r="B55" s="136"/>
-      <c r="C55" s="141"/>
-      <c r="D55" s="140"/>
-      <c r="E55" s="141" t="s">
-        <v>236</v>
-      </c>
-      <c r="F55" s="136"/>
-    </row>
-    <row r="56" spans="2:6" ht="18" customHeight="1">
-      <c r="B56" s="136"/>
-      <c r="C56" s="141"/>
-      <c r="D56" s="140"/>
-      <c r="E56" s="141" t="s">
-        <v>234</v>
-      </c>
-      <c r="F56" s="136"/>
-    </row>
-    <row r="57" spans="2:6" ht="18" customHeight="1">
-      <c r="B57" s="136"/>
-      <c r="C57" s="141"/>
-      <c r="D57" s="140"/>
-      <c r="E57" s="141" t="s">
-        <v>102</v>
-      </c>
-      <c r="F57" s="136"/>
-    </row>
-    <row r="58" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B58" s="136"/>
-      <c r="C58" s="141" t="s">
-        <v>217</v>
-      </c>
-      <c r="D58" s="136"/>
-      <c r="E58" s="141" t="s">
-        <v>216</v>
-      </c>
-      <c r="F58" s="141" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B59" s="136"/>
-      <c r="C59" s="141"/>
-      <c r="D59" s="136"/>
-      <c r="E59" s="141" t="s">
-        <v>219</v>
-      </c>
-      <c r="F59" s="141" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B60" s="136"/>
-      <c r="C60" s="136"/>
-      <c r="D60" s="136"/>
-      <c r="E60" s="141" t="s">
-        <v>222</v>
-      </c>
-      <c r="F60" s="141" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="61" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B61" s="136"/>
-      <c r="C61" s="136"/>
-      <c r="D61" s="141" t="s">
-        <v>223</v>
-      </c>
-      <c r="E61" s="136"/>
-      <c r="F61" s="141" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="62" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B62" s="136"/>
-      <c r="C62" s="136"/>
-      <c r="D62" s="136"/>
-      <c r="E62" s="141" t="s">
-        <v>95</v>
-      </c>
-      <c r="F62" s="136"/>
-    </row>
-    <row r="63" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B63" s="136"/>
-      <c r="C63" s="136"/>
-      <c r="D63" s="136"/>
-      <c r="E63" s="136" t="s">
-        <v>96</v>
-      </c>
-      <c r="F63" s="136"/>
-    </row>
-    <row r="64" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B64" s="136"/>
-      <c r="C64" s="136"/>
-      <c r="D64" s="136"/>
-      <c r="E64" s="141" t="s">
-        <v>97</v>
-      </c>
-      <c r="F64" s="141" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="65" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B65" s="136"/>
-      <c r="C65" s="141" t="s">
-        <v>225</v>
-      </c>
-      <c r="D65" s="141" t="s">
-        <v>226</v>
-      </c>
-      <c r="E65" s="136"/>
-      <c r="F65" s="141" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="66" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B66" s="136"/>
-      <c r="C66" s="136"/>
-      <c r="D66" s="136"/>
-      <c r="E66" s="141" t="s">
-        <v>230</v>
-      </c>
-      <c r="F66" s="136"/>
-    </row>
-    <row r="67" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B67" s="136"/>
-      <c r="C67" s="136"/>
-      <c r="D67" s="136"/>
-      <c r="E67" s="141" t="s">
-        <v>231</v>
-      </c>
-      <c r="F67" s="136"/>
-    </row>
-    <row r="68" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B68" s="136"/>
-      <c r="C68" s="136"/>
-      <c r="D68" s="141" t="s">
-        <v>223</v>
-      </c>
-      <c r="E68" s="136"/>
-      <c r="F68" s="141" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="69" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B69" s="136"/>
-      <c r="C69" s="136"/>
-      <c r="D69" s="136"/>
-      <c r="E69" s="141" t="s">
-        <v>97</v>
-      </c>
-      <c r="F69" s="141" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="70" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B70" s="136"/>
-      <c r="C70" s="141" t="s">
-        <v>241</v>
-      </c>
-      <c r="D70" s="141" t="s">
-        <v>243</v>
-      </c>
-      <c r="E70" s="136"/>
-      <c r="F70" s="141" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="71" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B71" s="136"/>
-      <c r="C71" s="136"/>
-      <c r="D71" s="136"/>
-      <c r="E71" s="141" t="s">
-        <v>244</v>
-      </c>
-      <c r="F71" s="136"/>
-    </row>
-    <row r="72" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B72" s="136"/>
-      <c r="C72" s="136"/>
-      <c r="D72" s="136"/>
-      <c r="E72" s="141" t="s">
-        <v>245</v>
-      </c>
-      <c r="F72" s="136"/>
-    </row>
-    <row r="73" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B73" s="136"/>
-      <c r="C73" s="136"/>
-      <c r="D73" s="136"/>
-      <c r="E73" s="141" t="s">
-        <v>246</v>
-      </c>
-      <c r="F73" s="136"/>
-    </row>
-    <row r="105" spans="4:4" ht="15.75" customHeight="1">
-      <c r="D105" t="s">
+      <c r="F71" s="157"/>
+    </row>
+    <row r="103" spans="4:4" ht="15.75" customHeight="1">
+      <c r="D103" t="s">
         <v>108</v>
       </c>
     </row>
@@ -4121,7 +4411,7 @@
   </sheetPr>
   <dimension ref="G1:W28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="CI1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -4297,13 +4587,13 @@
       <c r="J11" s="112"/>
       <c r="K11" s="112"/>
       <c r="L11" s="112"/>
-      <c r="M11" s="151"/>
-      <c r="N11" s="144"/>
-      <c r="O11" s="144"/>
+      <c r="M11" s="137"/>
+      <c r="N11" s="130"/>
+      <c r="O11" s="130"/>
       <c r="P11" s="112"/>
       <c r="Q11" s="112"/>
-      <c r="R11" s="151"/>
-      <c r="S11" s="152"/>
+      <c r="R11" s="137"/>
+      <c r="S11" s="138"/>
     </row>
     <row r="12" spans="7:19" ht="15">
       <c r="G12" s="38"/>
@@ -4509,9 +4799,9 @@
       <c r="W23" s="112"/>
     </row>
     <row r="24" spans="7:23" ht="15">
-      <c r="G24" s="150"/>
-      <c r="H24" s="144"/>
-      <c r="I24" s="144"/>
+      <c r="G24" s="136"/>
+      <c r="H24" s="130"/>
+      <c r="I24" s="130"/>
       <c r="J24" s="112"/>
       <c r="K24" s="112"/>
       <c r="L24" s="112"/>
@@ -4547,9 +4837,9 @@
       <c r="W25" s="112"/>
     </row>
     <row r="26" spans="7:23" ht="15">
-      <c r="G26" s="150"/>
-      <c r="H26" s="144"/>
-      <c r="I26" s="144"/>
+      <c r="G26" s="136"/>
+      <c r="H26" s="130"/>
+      <c r="I26" s="130"/>
       <c r="J26" s="112"/>
       <c r="K26" s="112"/>
       <c r="L26" s="112"/>
@@ -4594,14 +4884,14 @@
       <c r="M28" s="112"/>
       <c r="N28" s="112"/>
       <c r="O28" s="112"/>
-      <c r="P28" s="150"/>
-      <c r="Q28" s="144"/>
-      <c r="R28" s="144"/>
+      <c r="P28" s="136"/>
+      <c r="Q28" s="130"/>
+      <c r="R28" s="130"/>
       <c r="S28" s="112"/>
-      <c r="T28" s="150"/>
-      <c r="U28" s="144"/>
-      <c r="V28" s="144"/>
-      <c r="W28" s="144"/>
+      <c r="T28" s="136"/>
+      <c r="U28" s="130"/>
+      <c r="V28" s="130"/>
+      <c r="W28" s="130"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4643,14 +4933,14 @@
   <sheetData>
     <row r="1" spans="2:8" ht="87" customHeight="1">
       <c r="B1" s="110"/>
-      <c r="C1" s="148" t="s">
+      <c r="C1" s="134" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
     </row>
     <row r="2" spans="2:8" ht="12.75" customHeight="1">
       <c r="B2" s="112"/>
@@ -4773,12 +5063,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="64.5" customHeight="1">
-      <c r="C1" s="153" t="s">
+      <c r="C1" s="139" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="144"/>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
+      <c r="D1" s="130"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
     </row>
     <row r="2" spans="2:11" ht="13.2"/>
     <row r="3" spans="2:11" ht="13.2">
@@ -4801,10 +5091,10 @@
       <c r="E6" s="113"/>
     </row>
     <row r="7" spans="2:11" ht="26.4">
-      <c r="B7" s="154" t="s">
+      <c r="B7" s="140" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="144"/>
+      <c r="C7" s="130"/>
       <c r="G7" s="113" t="s">
         <v>133</v>
       </c>
@@ -4895,10 +5185,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:H11"/>
+  <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="88" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4907,7 +5197,7 @@
     <col min="2" max="2" width="38.5546875" customWidth="1"/>
     <col min="3" max="3" width="7.109375" customWidth="1"/>
     <col min="4" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
     <col min="8" max="8" width="16.5546875" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
@@ -4915,13 +5205,13 @@
     <row r="1" spans="2:8" ht="57" customHeight="1">
       <c r="B1" s="115"/>
       <c r="C1" s="116"/>
-      <c r="D1" s="153" t="s">
+      <c r="D1" s="139" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="144"/>
-      <c r="F1" s="144"/>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
+      <c r="E1" s="130"/>
+      <c r="F1" s="130"/>
+      <c r="G1" s="130"/>
+      <c r="H1" s="130"/>
     </row>
     <row r="2" spans="2:8" ht="12.75" customHeight="1">
       <c r="B2" s="115"/>
@@ -4991,48 +5281,293 @@
     </row>
     <row r="8" spans="2:8" ht="13.5" customHeight="1">
       <c r="C8" s="116"/>
-      <c r="D8" s="121" t="s">
+      <c r="D8" s="174" t="s">
         <v>155</v>
       </c>
-      <c r="E8" s="122"/>
-      <c r="F8" s="122"/>
-      <c r="G8" s="122"/>
-      <c r="H8" s="123"/>
+      <c r="E8" s="175" t="s">
+        <v>279</v>
+      </c>
+      <c r="F8" s="176" t="s">
+        <v>284</v>
+      </c>
+      <c r="G8" s="175"/>
+      <c r="H8" s="177"/>
     </row>
     <row r="9" spans="2:8" ht="14.25" customHeight="1">
       <c r="B9" s="115"/>
-      <c r="C9" s="124"/>
-      <c r="D9" s="125"/>
-      <c r="E9" s="126"/>
-      <c r="F9" s="126"/>
-      <c r="G9" s="126"/>
-      <c r="H9" s="127"/>
+      <c r="C9" s="121"/>
+      <c r="D9" s="178" t="s">
+        <v>241</v>
+      </c>
+      <c r="E9" s="167" t="s">
+        <v>279</v>
+      </c>
+      <c r="F9" s="179" t="s">
+        <v>284</v>
+      </c>
+      <c r="G9" s="180"/>
+      <c r="H9" s="181"/>
     </row>
     <row r="10" spans="2:8" ht="12.75" customHeight="1">
       <c r="B10" s="113" t="s">
         <v>156</v>
       </c>
       <c r="C10" s="116"/>
-      <c r="D10" s="128"/>
-      <c r="E10" s="129"/>
-      <c r="F10" s="129"/>
-      <c r="G10" s="129"/>
-      <c r="H10" s="130"/>
+      <c r="D10" s="166" t="s">
+        <v>184</v>
+      </c>
+      <c r="E10" s="168" t="s">
+        <v>279</v>
+      </c>
+      <c r="F10" s="167" t="s">
+        <v>284</v>
+      </c>
+      <c r="G10" s="168"/>
+      <c r="H10" s="169"/>
     </row>
     <row r="11" spans="2:8" ht="12.75" customHeight="1">
       <c r="B11" s="56" t="s">
         <v>157</v>
       </c>
       <c r="C11" s="116"/>
-      <c r="D11" s="128"/>
-      <c r="E11" s="129"/>
-      <c r="F11" s="129"/>
-      <c r="G11" s="129"/>
-      <c r="H11" s="130"/>
+      <c r="D11" s="166" t="s">
+        <v>267</v>
+      </c>
+      <c r="E11" s="167" t="s">
+        <v>279</v>
+      </c>
+      <c r="F11" s="167" t="s">
+        <v>284</v>
+      </c>
+      <c r="G11" s="168"/>
+      <c r="H11" s="169"/>
+    </row>
+    <row r="12" spans="2:8" ht="15.75" customHeight="1">
+      <c r="D12" s="166" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="168" t="s">
+        <v>279</v>
+      </c>
+      <c r="F12" s="167" t="s">
+        <v>284</v>
+      </c>
+      <c r="G12" s="168"/>
+      <c r="H12" s="169"/>
+    </row>
+    <row r="13" spans="2:8" ht="15.75" customHeight="1">
+      <c r="D13" s="166" t="s">
+        <v>268</v>
+      </c>
+      <c r="E13" s="168" t="s">
+        <v>279</v>
+      </c>
+      <c r="F13" s="167" t="s">
+        <v>284</v>
+      </c>
+      <c r="G13" s="168"/>
+      <c r="H13" s="169"/>
+    </row>
+    <row r="14" spans="2:8" ht="15.75" customHeight="1">
+      <c r="D14" s="166" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="168" t="s">
+        <v>279</v>
+      </c>
+      <c r="F14" s="167" t="s">
+        <v>284</v>
+      </c>
+      <c r="G14" s="168"/>
+      <c r="H14" s="169"/>
+    </row>
+    <row r="15" spans="2:8" ht="15.75" customHeight="1">
+      <c r="D15" s="166" t="s">
+        <v>182</v>
+      </c>
+      <c r="E15" s="167" t="s">
+        <v>279</v>
+      </c>
+      <c r="F15" s="167" t="s">
+        <v>284</v>
+      </c>
+      <c r="G15" s="168"/>
+      <c r="H15" s="169"/>
+    </row>
+    <row r="16" spans="2:8" ht="15.75" customHeight="1">
+      <c r="D16" s="170" t="s">
+        <v>280</v>
+      </c>
+      <c r="E16" s="171"/>
+      <c r="F16" s="171"/>
+      <c r="G16" s="171"/>
+      <c r="H16" s="172"/>
+    </row>
+    <row r="17" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D17" s="178" t="s">
+        <v>278</v>
+      </c>
+      <c r="E17" s="184" t="s">
+        <v>279</v>
+      </c>
+      <c r="F17" s="173" t="s">
+        <v>285</v>
+      </c>
+      <c r="G17" s="168"/>
+      <c r="H17" s="183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D18" s="178" t="s">
+        <v>281</v>
+      </c>
+      <c r="E18" s="184" t="s">
+        <v>279</v>
+      </c>
+      <c r="F18" s="173" t="s">
+        <v>285</v>
+      </c>
+      <c r="G18" s="168"/>
+      <c r="H18" s="183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D19" s="178" t="s">
+        <v>282</v>
+      </c>
+      <c r="E19" s="184" t="s">
+        <v>279</v>
+      </c>
+      <c r="F19" s="173" t="s">
+        <v>286</v>
+      </c>
+      <c r="G19" s="168"/>
+      <c r="H19" s="183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D20" s="178" t="s">
+        <v>283</v>
+      </c>
+      <c r="E20" s="184" t="s">
+        <v>279</v>
+      </c>
+      <c r="F20" s="173" t="s">
+        <v>286</v>
+      </c>
+      <c r="G20" s="168"/>
+      <c r="H20" s="185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D21" s="178" t="s">
+        <v>287</v>
+      </c>
+      <c r="E21" s="182" t="s">
+        <v>288</v>
+      </c>
+      <c r="F21" s="167" t="s">
+        <v>286</v>
+      </c>
+      <c r="G21" s="168"/>
+      <c r="H21" s="185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D22" s="178" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="182" t="s">
+        <v>288</v>
+      </c>
+      <c r="F22" s="167" t="s">
+        <v>289</v>
+      </c>
+      <c r="G22" s="168"/>
+      <c r="H22" s="185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D23" s="178" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="182" t="s">
+        <v>288</v>
+      </c>
+      <c r="F23" s="167" t="s">
+        <v>289</v>
+      </c>
+      <c r="G23" s="168"/>
+      <c r="H23" s="185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D24" s="166"/>
+      <c r="E24" s="168"/>
+      <c r="F24" s="168"/>
+      <c r="G24" s="168"/>
+      <c r="H24" s="169"/>
+    </row>
+    <row r="25" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D25" s="166"/>
+      <c r="E25" s="168"/>
+      <c r="F25" s="168"/>
+      <c r="G25" s="168"/>
+      <c r="H25" s="169"/>
+    </row>
+    <row r="26" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D26" s="166"/>
+      <c r="E26" s="168"/>
+      <c r="F26" s="168"/>
+      <c r="G26" s="168"/>
+      <c r="H26" s="169"/>
+    </row>
+    <row r="27" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D27" s="166"/>
+      <c r="E27" s="168"/>
+      <c r="F27" s="168"/>
+      <c r="G27" s="168"/>
+      <c r="H27" s="169"/>
+    </row>
+    <row r="28" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D28" s="166"/>
+      <c r="E28" s="168"/>
+      <c r="F28" s="168"/>
+      <c r="G28" s="168"/>
+      <c r="H28" s="169"/>
+    </row>
+    <row r="29" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D29" s="166"/>
+      <c r="E29" s="168"/>
+      <c r="F29" s="168"/>
+      <c r="G29" s="168"/>
+      <c r="H29" s="169"/>
+    </row>
+    <row r="30" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D30" s="166"/>
+      <c r="E30" s="168"/>
+      <c r="F30" s="168"/>
+      <c r="G30" s="168"/>
+      <c r="H30" s="169"/>
+    </row>
+    <row r="31" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D31" s="166"/>
+      <c r="E31" s="168"/>
+      <c r="F31" s="168"/>
+      <c r="G31" s="168"/>
+      <c r="H31" s="169"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D1:H1"/>
+    <mergeCell ref="D16:H16"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
@@ -5087,12 +5622,12 @@
       <c r="E3" s="71"/>
       <c r="F3" s="71"/>
       <c r="G3" s="71"/>
-      <c r="H3" s="155"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="144"/>
-      <c r="M3" s="144"/>
+      <c r="H3" s="141"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="130"/>
     </row>
     <row r="4" spans="2:13" ht="21.75" customHeight="1">
       <c r="B4" s="102"/>
@@ -5200,7 +5735,7 @@
       <c r="B10" s="84" t="s">
         <v>168</v>
       </c>
-      <c r="C10" s="131" t="s">
+      <c r="C10" s="122" t="s">
         <v>169</v>
       </c>
       <c r="D10" s="86" t="s">
@@ -5544,18 +6079,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5578,18 +6113,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8039DF66-AB83-49D2-BABD-681C7E045BB6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B130DE0C-7A28-4B03-98EC-F451E5EF5DFD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8039DF66-AB83-49D2-BABD-681C7E045BB6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
pas reussi mais presque je crois
</commit_message>
<xml_diff>
--- a/Gestion_A_jmd.xlsx
+++ b/Gestion_A_jmd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dilio\OneDrive\Bureau\ProjetDaleks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ouaiouaihashish\Desktop\ProjetDaleks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{745BF8D5-3E86-44F5-9CD9-AAD9AAA3DBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D30532-572E-4940-A228-F9578A94228A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Méthodes SCRUM" sheetId="1" r:id="rId1"/>
@@ -976,9 +976,6 @@
     <t>Position dalek</t>
   </si>
   <si>
-    <t>Position aéleatoir sauf même case</t>
-  </si>
-  <si>
     <t>coordonée x y (différente)</t>
   </si>
   <si>
@@ -1109,6 +1106,9 @@
   </si>
   <si>
     <t>2h</t>
+  </si>
+  <si>
+    <t>Position aléatoir sauf même case</t>
   </si>
 </sst>
 </file>
@@ -2216,6 +2216,120 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="51" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="3" borderId="51" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="5" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="11" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="12" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2250,133 +2364,19 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="51" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="3" borderId="51" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="51" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="11" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="12" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2724,17 +2724,17 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" customWidth="1"/>
-    <col min="3" max="3" width="44.33203125" customWidth="1"/>
-    <col min="4" max="4" width="69.44140625" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" customWidth="1"/>
-    <col min="7" max="7" width="45.33203125" customWidth="1"/>
-    <col min="8" max="8" width="67.88671875" customWidth="1"/>
-    <col min="9" max="28" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="3" max="3" width="44.28515625" customWidth="1"/>
+    <col min="4" max="4" width="69.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.5703125" customWidth="1"/>
+    <col min="7" max="7" width="45.28515625" customWidth="1"/>
+    <col min="8" max="8" width="67.85546875" customWidth="1"/>
+    <col min="9" max="28" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="17.25" customHeight="1">
@@ -3077,22 +3077,22 @@
       </c>
     </row>
     <row r="36" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F36" s="129"/>
-      <c r="G36" s="130"/>
-      <c r="H36" s="130"/>
-      <c r="I36" s="130"/>
+      <c r="F36" s="169"/>
+      <c r="G36" s="170"/>
+      <c r="H36" s="170"/>
+      <c r="I36" s="170"/>
     </row>
     <row r="37" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F37" s="130"/>
-      <c r="G37" s="130"/>
-      <c r="H37" s="130"/>
-      <c r="I37" s="130"/>
+      <c r="F37" s="170"/>
+      <c r="G37" s="170"/>
+      <c r="H37" s="170"/>
+      <c r="I37" s="170"/>
     </row>
     <row r="38" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F38" s="130"/>
-      <c r="G38" s="130"/>
-      <c r="H38" s="130"/>
-      <c r="I38" s="130"/>
+      <c r="F38" s="170"/>
+      <c r="G38" s="170"/>
+      <c r="H38" s="170"/>
+      <c r="I38" s="170"/>
     </row>
     <row r="39" spans="6:9" ht="17.25" customHeight="1">
       <c r="F39" s="112"/>
@@ -3101,22 +3101,22 @@
       <c r="I39" s="112"/>
     </row>
     <row r="40" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F40" s="129"/>
-      <c r="G40" s="130"/>
-      <c r="H40" s="130"/>
-      <c r="I40" s="130"/>
+      <c r="F40" s="169"/>
+      <c r="G40" s="170"/>
+      <c r="H40" s="170"/>
+      <c r="I40" s="170"/>
     </row>
     <row r="41" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F41" s="130"/>
-      <c r="G41" s="130"/>
-      <c r="H41" s="130"/>
-      <c r="I41" s="130"/>
+      <c r="F41" s="170"/>
+      <c r="G41" s="170"/>
+      <c r="H41" s="170"/>
+      <c r="I41" s="170"/>
     </row>
     <row r="42" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F42" s="130"/>
-      <c r="G42" s="130"/>
-      <c r="H42" s="130"/>
-      <c r="I42" s="130"/>
+      <c r="F42" s="170"/>
+      <c r="G42" s="170"/>
+      <c r="H42" s="170"/>
+      <c r="I42" s="170"/>
     </row>
     <row r="43" spans="6:9" ht="17.25" customHeight="1">
       <c r="F43" s="112"/>
@@ -3131,34 +3131,34 @@
       <c r="I44" s="112"/>
     </row>
     <row r="45" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F45" s="129"/>
-      <c r="G45" s="130"/>
-      <c r="H45" s="130"/>
-      <c r="I45" s="130"/>
+      <c r="F45" s="169"/>
+      <c r="G45" s="170"/>
+      <c r="H45" s="170"/>
+      <c r="I45" s="170"/>
     </row>
     <row r="46" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F46" s="130"/>
-      <c r="G46" s="130"/>
-      <c r="H46" s="130"/>
-      <c r="I46" s="130"/>
+      <c r="F46" s="170"/>
+      <c r="G46" s="170"/>
+      <c r="H46" s="170"/>
+      <c r="I46" s="170"/>
     </row>
     <row r="47" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F47" s="130"/>
-      <c r="G47" s="130"/>
-      <c r="H47" s="130"/>
-      <c r="I47" s="130"/>
+      <c r="F47" s="170"/>
+      <c r="G47" s="170"/>
+      <c r="H47" s="170"/>
+      <c r="I47" s="170"/>
     </row>
     <row r="48" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F48" s="130"/>
-      <c r="G48" s="130"/>
-      <c r="H48" s="130"/>
-      <c r="I48" s="130"/>
+      <c r="F48" s="170"/>
+      <c r="G48" s="170"/>
+      <c r="H48" s="170"/>
+      <c r="I48" s="170"/>
     </row>
     <row r="49" spans="6:9" ht="17.25" customHeight="1">
-      <c r="F49" s="130"/>
-      <c r="G49" s="130"/>
-      <c r="H49" s="130"/>
-      <c r="I49" s="130"/>
+      <c r="F49" s="170"/>
+      <c r="G49" s="170"/>
+      <c r="H49" s="170"/>
+      <c r="I49" s="170"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3177,18 +3177,18 @@
   </sheetPr>
   <dimension ref="B2:E46"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="66" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="37.88671875" customWidth="1"/>
-    <col min="3" max="3" width="37.33203125" customWidth="1"/>
-    <col min="4" max="4" width="138.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="138.7109375" customWidth="1"/>
     <col min="5" max="5" width="48" customWidth="1"/>
-    <col min="6" max="7" width="8.5546875" customWidth="1"/>
+    <col min="6" max="7" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="12.75" customHeight="1">
@@ -3280,7 +3280,7 @@
       </c>
     </row>
     <row r="13" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B13" s="131" t="s">
+      <c r="B13" s="171" t="s">
         <v>60</v>
       </c>
       <c r="C13" s="16" t="s">
@@ -3294,7 +3294,7 @@
       </c>
     </row>
     <row r="14" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B14" s="132"/>
+      <c r="B14" s="172"/>
       <c r="C14" s="22" t="s">
         <v>63</v>
       </c>
@@ -3306,7 +3306,7 @@
       </c>
     </row>
     <row r="15" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B15" s="132"/>
+      <c r="B15" s="172"/>
       <c r="C15" s="22" t="s">
         <v>65</v>
       </c>
@@ -3318,19 +3318,19 @@
       </c>
     </row>
     <row r="16" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B16" s="132"/>
+      <c r="B16" s="172"/>
       <c r="C16" s="126" t="s">
         <v>211</v>
       </c>
       <c r="D16" s="125" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E16" s="41" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B17" s="132"/>
+      <c r="B17" s="172"/>
       <c r="C17" s="22" t="s">
         <v>67</v>
       </c>
@@ -3342,7 +3342,7 @@
       </c>
     </row>
     <row r="18" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B18" s="132"/>
+      <c r="B18" s="172"/>
       <c r="C18" s="22" t="s">
         <v>182</v>
       </c>
@@ -3352,7 +3352,7 @@
       <c r="E18" s="41"/>
     </row>
     <row r="19" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B19" s="132"/>
+      <c r="B19" s="172"/>
       <c r="C19" s="22" t="s">
         <v>69</v>
       </c>
@@ -3360,11 +3360,11 @@
         <v>70</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B20" s="132"/>
+      <c r="B20" s="172"/>
       <c r="C20" s="22" t="s">
         <v>241</v>
       </c>
@@ -3376,72 +3376,72 @@
       </c>
     </row>
     <row r="21" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B21" s="132"/>
+      <c r="B21" s="172"/>
       <c r="C21" s="22" t="s">
         <v>91</v>
       </c>
       <c r="D21" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="E21" s="41" t="s">
         <v>250</v>
       </c>
-      <c r="E21" s="41" t="s">
-        <v>251</v>
-      </c>
     </row>
     <row r="22" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B22" s="132"/>
+      <c r="B22" s="172"/>
       <c r="C22" s="22" t="s">
         <v>71</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E22" s="124" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="23" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B23" s="132"/>
+      <c r="B23" s="172"/>
       <c r="C23" s="22" t="s">
+        <v>255</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>258</v>
+      </c>
+      <c r="E23" s="124" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="12.75" customHeight="1">
+      <c r="B24" s="172"/>
+      <c r="C24" s="22" t="s">
         <v>256</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D24" s="18" t="s">
         <v>259</v>
       </c>
-      <c r="E23" s="124" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B24" s="132"/>
-      <c r="C24" s="22" t="s">
+      <c r="E24" s="124" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="12.75" customHeight="1">
+      <c r="B25" s="172"/>
+      <c r="C25" s="22" t="s">
         <v>257</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D25" s="18" t="s">
         <v>260</v>
       </c>
-      <c r="E24" s="124" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B25" s="132"/>
-      <c r="C25" s="22" t="s">
-        <v>258</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>261</v>
-      </c>
       <c r="E25" s="124" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B26" s="133"/>
+      <c r="B26" s="173"/>
       <c r="C26" s="19" t="s">
         <v>73</v>
       </c>
       <c r="D26" s="40" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E26" s="123" t="s">
         <v>206</v>
@@ -3450,17 +3450,17 @@
     <row r="27" spans="2:5" ht="12.75" customHeight="1">
       <c r="B27" s="108"/>
       <c r="C27" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="E27" s="124" t="s">
         <v>265</v>
       </c>
-      <c r="E27" s="124" t="s">
-        <v>266</v>
-      </c>
     </row>
     <row r="28" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B28" s="131" t="s">
+      <c r="B28" s="171" t="s">
         <v>75</v>
       </c>
       <c r="C28" s="23" t="s">
@@ -3474,135 +3474,135 @@
       </c>
     </row>
     <row r="29" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B29" s="132"/>
+      <c r="B29" s="172"/>
       <c r="C29" s="22" t="s">
         <v>244</v>
       </c>
       <c r="D29" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="E29" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="E29" s="41" t="s">
-        <v>246</v>
-      </c>
     </row>
     <row r="30" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B30" s="132"/>
+      <c r="B30" s="172"/>
       <c r="C30" s="22" t="s">
         <v>61</v>
       </c>
       <c r="D30" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="E30" s="41" t="s">
         <v>252</v>
       </c>
-      <c r="E30" s="41" t="s">
-        <v>253</v>
-      </c>
     </row>
     <row r="31" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B31" s="132"/>
+      <c r="B31" s="172"/>
       <c r="C31" s="22" t="s">
         <v>71</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B32" s="132"/>
+      <c r="B32" s="172"/>
       <c r="C32" s="22"/>
       <c r="D32" s="18"/>
       <c r="E32" s="41"/>
     </row>
     <row r="33" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B33" s="132"/>
+      <c r="B33" s="172"/>
       <c r="C33" s="22"/>
       <c r="D33" s="18"/>
       <c r="E33" s="41"/>
     </row>
     <row r="34" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B34" s="132"/>
+      <c r="B34" s="172"/>
       <c r="C34" s="22"/>
       <c r="D34" s="18"/>
       <c r="E34" s="41"/>
     </row>
     <row r="35" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B35" s="132"/>
+      <c r="B35" s="172"/>
       <c r="C35" s="22"/>
       <c r="D35" s="18"/>
       <c r="E35" s="41"/>
     </row>
     <row r="36" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B36" s="133"/>
+      <c r="B36" s="173"/>
       <c r="C36" s="19"/>
       <c r="D36" s="40"/>
       <c r="E36" s="20"/>
     </row>
     <row r="37" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B37" s="131" t="s">
+      <c r="B37" s="171" t="s">
         <v>76</v>
       </c>
       <c r="C37" s="23" t="s">
+        <v>246</v>
+      </c>
+      <c r="D37" s="39" t="s">
         <v>247</v>
       </c>
-      <c r="D37" s="39" t="s">
+      <c r="E37" s="21" t="s">
         <v>248</v>
       </c>
-      <c r="E37" s="21" t="s">
-        <v>249</v>
-      </c>
     </row>
     <row r="38" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B38" s="132"/>
+      <c r="B38" s="172"/>
       <c r="C38" s="22"/>
       <c r="D38" s="18"/>
       <c r="E38" s="41"/>
     </row>
     <row r="39" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B39" s="132"/>
+      <c r="B39" s="172"/>
       <c r="C39" s="22"/>
       <c r="D39" s="18"/>
       <c r="E39" s="41"/>
     </row>
     <row r="40" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B40" s="132"/>
+      <c r="B40" s="172"/>
       <c r="C40" s="22"/>
       <c r="D40" s="18"/>
       <c r="E40" s="41"/>
     </row>
     <row r="41" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B41" s="132"/>
+      <c r="B41" s="172"/>
       <c r="C41" s="22"/>
       <c r="D41" s="18"/>
       <c r="E41" s="41"/>
     </row>
     <row r="42" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B42" s="132"/>
+      <c r="B42" s="172"/>
       <c r="C42" s="22"/>
       <c r="D42" s="18"/>
       <c r="E42" s="41"/>
     </row>
     <row r="43" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B43" s="132"/>
+      <c r="B43" s="172"/>
       <c r="C43" s="22"/>
       <c r="D43" s="18"/>
       <c r="E43" s="41"/>
     </row>
     <row r="44" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B44" s="132"/>
+      <c r="B44" s="172"/>
       <c r="C44" s="22"/>
       <c r="D44" s="18"/>
       <c r="E44" s="41"/>
     </row>
     <row r="45" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B45" s="132"/>
+      <c r="B45" s="172"/>
       <c r="C45" s="22"/>
       <c r="D45" s="18"/>
       <c r="E45" s="41"/>
     </row>
     <row r="46" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B46" s="133"/>
+      <c r="B46" s="173"/>
       <c r="C46" s="24"/>
       <c r="D46" s="25"/>
       <c r="E46" s="46"/>
@@ -3624,19 +3624,19 @@
   </sheetPr>
   <dimension ref="B2:F103"/>
   <sheetViews>
-    <sheetView topLeftCell="F9" zoomScale="75" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView topLeftCell="A27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" customWidth="1"/>
-    <col min="3" max="3" width="34.109375" customWidth="1"/>
-    <col min="4" max="4" width="44.44140625" customWidth="1"/>
-    <col min="5" max="5" width="49.5546875" customWidth="1"/>
-    <col min="6" max="6" width="138.6640625" customWidth="1"/>
-    <col min="7" max="8" width="17.6640625" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" customWidth="1"/>
+    <col min="5" max="5" width="49.5703125" customWidth="1"/>
+    <col min="6" max="6" width="138.7109375" customWidth="1"/>
+    <col min="7" max="8" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="20.25" customHeight="1">
@@ -3648,22 +3648,22 @@
       <c r="E2" s="109"/>
       <c r="F2" s="109"/>
     </row>
-    <row r="3" spans="2:6" ht="89.4" customHeight="1">
+    <row r="3" spans="2:6" ht="89.45" customHeight="1">
       <c r="B3" s="109"/>
-      <c r="C3" s="134" t="s">
+      <c r="C3" s="174" t="s">
         <v>78</v>
       </c>
-      <c r="D3" s="130"/>
-      <c r="E3" s="130"/>
+      <c r="D3" s="170"/>
+      <c r="E3" s="170"/>
       <c r="F3" s="109"/>
     </row>
     <row r="4" spans="2:6" ht="30.75" customHeight="1">
       <c r="B4" s="110"/>
-      <c r="C4" s="135" t="s">
+      <c r="C4" s="175" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="130"/>
-      <c r="E4" s="130"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
       <c r="F4" s="110"/>
     </row>
     <row r="5" spans="2:6" ht="21" customHeight="1">
@@ -3743,62 +3743,62 @@
       <c r="D12" s="32"/>
     </row>
     <row r="13" spans="2:6" ht="18" customHeight="1">
-      <c r="B13" s="142" t="s">
+      <c r="B13" s="129" t="s">
         <v>91</v>
       </c>
-      <c r="C13" s="159" t="s">
+      <c r="C13" s="146" t="s">
         <v>187</v>
       </c>
-      <c r="D13" s="143" t="s">
+      <c r="D13" s="130" t="s">
         <v>92</v>
       </c>
-      <c r="E13" s="142"/>
-      <c r="F13" s="142"/>
+      <c r="E13" s="129"/>
+      <c r="F13" s="129"/>
     </row>
     <row r="14" spans="2:6" ht="18" customHeight="1">
-      <c r="B14" s="144"/>
-      <c r="C14" s="145"/>
-      <c r="D14" s="144"/>
-      <c r="E14" s="146" t="s">
+      <c r="B14" s="131"/>
+      <c r="C14" s="132"/>
+      <c r="D14" s="131"/>
+      <c r="E14" s="133" t="s">
         <v>93</v>
       </c>
-      <c r="F14" s="142"/>
+      <c r="F14" s="129"/>
     </row>
     <row r="15" spans="2:6" ht="18" customHeight="1">
-      <c r="B15" s="144"/>
-      <c r="C15" s="147"/>
-      <c r="D15" s="144"/>
-      <c r="E15" s="146" t="s">
+      <c r="B15" s="131"/>
+      <c r="C15" s="134"/>
+      <c r="D15" s="131"/>
+      <c r="E15" s="133" t="s">
         <v>94</v>
       </c>
-      <c r="F15" s="146"/>
+      <c r="F15" s="133"/>
     </row>
     <row r="16" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B16" s="142"/>
-      <c r="C16" s="142"/>
-      <c r="D16" s="142"/>
-      <c r="E16" s="146" t="s">
+      <c r="B16" s="129"/>
+      <c r="C16" s="129"/>
+      <c r="D16" s="129"/>
+      <c r="E16" s="133" t="s">
         <v>95</v>
       </c>
-      <c r="F16" s="142"/>
+      <c r="F16" s="129"/>
     </row>
     <row r="17" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B17" s="142"/>
-      <c r="C17" s="142"/>
-      <c r="D17" s="146"/>
-      <c r="E17" s="142" t="s">
+      <c r="B17" s="129"/>
+      <c r="C17" s="129"/>
+      <c r="D17" s="133"/>
+      <c r="E17" s="129" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="142"/>
+      <c r="F17" s="129"/>
     </row>
     <row r="18" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B18" s="142"/>
-      <c r="C18" s="142"/>
-      <c r="D18" s="142"/>
-      <c r="E18" s="146" t="s">
+      <c r="B18" s="129"/>
+      <c r="C18" s="129"/>
+      <c r="D18" s="129"/>
+      <c r="E18" s="133" t="s">
         <v>97</v>
       </c>
-      <c r="F18" s="146" t="s">
+      <c r="F18" s="133" t="s">
         <v>189</v>
       </c>
     </row>
@@ -3806,7 +3806,7 @@
       <c r="B19" s="127" t="s">
         <v>91</v>
       </c>
-      <c r="C19" s="160" t="s">
+      <c r="C19" s="147" t="s">
         <v>98</v>
       </c>
       <c r="D19" s="128" t="s">
@@ -3849,7 +3849,7 @@
       <c r="C23" s="127"/>
       <c r="D23" s="128"/>
       <c r="E23" s="128" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F23" s="128"/>
     </row>
@@ -3863,7 +3863,7 @@
         <v>190</v>
       </c>
       <c r="F24" s="128" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="25" spans="2:6" ht="15.75" customHeight="1">
@@ -3922,472 +3922,472 @@
       </c>
     </row>
     <row r="30" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B30" s="148" t="s">
+      <c r="B30" s="135" t="s">
         <v>91</v>
       </c>
-      <c r="C30" s="161" t="s">
+      <c r="C30" s="148" t="s">
         <v>104</v>
       </c>
-      <c r="D30" s="148"/>
-      <c r="E30" s="148"/>
-      <c r="F30" s="149" t="s">
+      <c r="D30" s="135"/>
+      <c r="E30" s="135"/>
+      <c r="F30" s="136" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B31" s="148"/>
-      <c r="C31" s="148"/>
-      <c r="D31" s="149"/>
-      <c r="E31" s="149" t="s">
+      <c r="B31" s="135"/>
+      <c r="C31" s="135"/>
+      <c r="D31" s="136"/>
+      <c r="E31" s="136" t="s">
         <v>194</v>
       </c>
-      <c r="F31" s="149" t="s">
+      <c r="F31" s="136" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="32" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B32" s="148"/>
-      <c r="C32" s="148"/>
-      <c r="D32" s="149"/>
-      <c r="E32" s="148" t="s">
+      <c r="B32" s="135"/>
+      <c r="C32" s="135"/>
+      <c r="D32" s="136"/>
+      <c r="E32" s="135" t="s">
         <v>107</v>
       </c>
-      <c r="F32" s="149"/>
+      <c r="F32" s="136"/>
     </row>
     <row r="33" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B33" s="148"/>
-      <c r="C33" s="148"/>
-      <c r="D33" s="149"/>
-      <c r="E33" s="149" t="s">
+      <c r="B33" s="135"/>
+      <c r="C33" s="135"/>
+      <c r="D33" s="136"/>
+      <c r="E33" s="136" t="s">
         <v>195</v>
       </c>
-      <c r="F33" s="149" t="s">
+      <c r="F33" s="136" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B34" s="148" t="s">
+      <c r="B34" s="135" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="161" t="s">
+      <c r="C34" s="148" t="s">
         <v>198</v>
       </c>
-      <c r="D34" s="148"/>
-      <c r="E34" s="149" t="s">
+      <c r="D34" s="135"/>
+      <c r="E34" s="136" t="s">
+        <v>268</v>
+      </c>
+      <c r="F34" s="136" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B35" s="135"/>
+      <c r="C35" s="135"/>
+      <c r="D35" s="135"/>
+      <c r="E35" s="136" t="s">
         <v>269</v>
       </c>
-      <c r="F34" s="149" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="35" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B35" s="148"/>
-      <c r="C35" s="148"/>
-      <c r="D35" s="148"/>
-      <c r="E35" s="149" t="s">
+      <c r="F35" s="136" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B36" s="135"/>
+      <c r="C36" s="135"/>
+      <c r="D36" s="135"/>
+      <c r="E36" s="136" t="s">
         <v>270</v>
       </c>
-      <c r="F35" s="149" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="36" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B36" s="148"/>
-      <c r="C36" s="148"/>
-      <c r="D36" s="148"/>
-      <c r="E36" s="149" t="s">
-        <v>271</v>
-      </c>
-      <c r="F36" s="149" t="s">
+      <c r="F36" s="136" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="37" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B37" s="148"/>
-      <c r="C37" s="148"/>
-      <c r="D37" s="148"/>
-      <c r="E37" s="149" t="s">
+      <c r="B37" s="135"/>
+      <c r="C37" s="135"/>
+      <c r="D37" s="135"/>
+      <c r="E37" s="136" t="s">
         <v>231</v>
       </c>
-      <c r="F37" s="149" t="s">
+      <c r="F37" s="136" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="38" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B38" s="148"/>
-      <c r="C38" s="148"/>
-      <c r="D38" s="148"/>
-      <c r="E38" s="149" t="s">
+      <c r="B38" s="135"/>
+      <c r="C38" s="135"/>
+      <c r="D38" s="135"/>
+      <c r="E38" s="136" t="s">
         <v>229</v>
       </c>
-      <c r="F38" s="149" t="s">
+      <c r="F38" s="136" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="39" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B39" s="148"/>
-      <c r="C39" s="148"/>
-      <c r="D39" s="148"/>
-      <c r="E39" s="149" t="s">
+      <c r="B39" s="135"/>
+      <c r="C39" s="135"/>
+      <c r="D39" s="135"/>
+      <c r="E39" s="136" t="s">
         <v>102</v>
       </c>
-      <c r="F39" s="149"/>
+      <c r="F39" s="136"/>
     </row>
     <row r="40" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B40" s="150" t="s">
+      <c r="B40" s="137" t="s">
         <v>91</v>
       </c>
-      <c r="C40" s="162" t="s">
+      <c r="C40" s="149" t="s">
         <v>72</v>
       </c>
-      <c r="D40" s="151" t="s">
+      <c r="D40" s="138" t="s">
         <v>105</v>
       </c>
-      <c r="E40" s="150"/>
-      <c r="F40" s="151" t="s">
-        <v>276</v>
+      <c r="E40" s="137"/>
+      <c r="F40" s="138" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="41" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B41" s="150"/>
-      <c r="C41" s="150"/>
-      <c r="D41" s="150"/>
-      <c r="E41" s="151" t="s">
+      <c r="B41" s="137"/>
+      <c r="C41" s="137"/>
+      <c r="D41" s="137"/>
+      <c r="E41" s="138" t="s">
         <v>202</v>
       </c>
-      <c r="F41" s="151" t="s">
+      <c r="F41" s="138" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="42" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B42" s="150"/>
-      <c r="C42" s="150"/>
-      <c r="D42" s="150"/>
-      <c r="E42" s="150" t="s">
+      <c r="B42" s="137"/>
+      <c r="C42" s="137"/>
+      <c r="D42" s="137"/>
+      <c r="E42" s="137" t="s">
         <v>107</v>
       </c>
-      <c r="F42" s="151"/>
+      <c r="F42" s="138"/>
     </row>
     <row r="43" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B43" s="150" t="s">
+      <c r="B43" s="137" t="s">
         <v>89</v>
       </c>
-      <c r="C43" s="162" t="s">
+      <c r="C43" s="149" t="s">
         <v>204</v>
       </c>
-      <c r="D43" s="150"/>
-      <c r="E43" s="151" t="s">
+      <c r="D43" s="137"/>
+      <c r="E43" s="138" t="s">
+        <v>268</v>
+      </c>
+      <c r="F43" s="138" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B44" s="137"/>
+      <c r="C44" s="138"/>
+      <c r="D44" s="137"/>
+      <c r="E44" s="138" t="s">
         <v>269</v>
       </c>
-      <c r="F43" s="151" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="44" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B44" s="150"/>
-      <c r="C44" s="151"/>
-      <c r="D44" s="150"/>
-      <c r="E44" s="151" t="s">
+      <c r="F44" s="138" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B45" s="137"/>
+      <c r="C45" s="138"/>
+      <c r="D45" s="137"/>
+      <c r="E45" s="138" t="s">
         <v>270</v>
       </c>
-      <c r="F44" s="151" t="s">
+      <c r="F45" s="138" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B46" s="137"/>
+      <c r="C46" s="138"/>
+      <c r="D46" s="137"/>
+      <c r="E46" s="138" t="s">
+        <v>272</v>
+      </c>
+      <c r="F46" s="137"/>
+    </row>
+    <row r="47" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B47" s="137"/>
+      <c r="C47" s="138"/>
+      <c r="D47" s="137"/>
+      <c r="E47" s="138" t="s">
+        <v>102</v>
+      </c>
+      <c r="F47" s="137"/>
+    </row>
+    <row r="48" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B48" s="139" t="s">
+        <v>91</v>
+      </c>
+      <c r="C48" s="150" t="s">
+        <v>205</v>
+      </c>
+      <c r="D48" s="140" t="s">
+        <v>105</v>
+      </c>
+      <c r="E48" s="139"/>
+      <c r="F48" s="140" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B49" s="139"/>
+      <c r="C49" s="139"/>
+      <c r="D49" s="139"/>
+      <c r="E49" s="140" t="s">
+        <v>208</v>
+      </c>
+      <c r="F49" s="140" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B50" s="139"/>
+      <c r="C50" s="139"/>
+      <c r="D50" s="139"/>
+      <c r="E50" s="140" t="s">
+        <v>231</v>
+      </c>
+      <c r="F50" s="140" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B51" s="139"/>
+      <c r="C51" s="139"/>
+      <c r="D51" s="139"/>
+      <c r="E51" s="140" t="s">
+        <v>195</v>
+      </c>
+      <c r="F51" s="140"/>
+    </row>
+    <row r="52" spans="2:6" ht="18" customHeight="1">
+      <c r="B52" s="139" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" s="150" t="s">
+        <v>198</v>
+      </c>
+      <c r="D52" s="141"/>
+      <c r="E52" s="140" t="s">
+        <v>268</v>
+      </c>
+      <c r="F52" s="140" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" ht="18" customHeight="1">
+      <c r="B53" s="139"/>
+      <c r="C53" s="140"/>
+      <c r="D53" s="141"/>
+      <c r="E53" s="140" t="s">
+        <v>269</v>
+      </c>
+      <c r="F53" s="140" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="45" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B45" s="150"/>
-      <c r="C45" s="151"/>
-      <c r="D45" s="150"/>
-      <c r="E45" s="151" t="s">
-        <v>271</v>
-      </c>
-      <c r="F45" s="151" t="s">
+    <row r="54" spans="2:6" ht="18" customHeight="1">
+      <c r="B54" s="139"/>
+      <c r="C54" s="140"/>
+      <c r="D54" s="141"/>
+      <c r="E54" s="140" t="s">
+        <v>272</v>
+      </c>
+      <c r="F54" s="140" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="46" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B46" s="150"/>
-      <c r="C46" s="151"/>
-      <c r="D46" s="150"/>
-      <c r="E46" s="151" t="s">
-        <v>273</v>
-      </c>
-      <c r="F46" s="150"/>
-    </row>
-    <row r="47" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B47" s="150"/>
-      <c r="C47" s="151"/>
-      <c r="D47" s="150"/>
-      <c r="E47" s="151" t="s">
+    <row r="55" spans="2:6" ht="18" customHeight="1">
+      <c r="B55" s="139"/>
+      <c r="C55" s="140"/>
+      <c r="D55" s="141"/>
+      <c r="E55" s="140" t="s">
         <v>102</v>
       </c>
-      <c r="F47" s="150"/>
-    </row>
-    <row r="48" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B48" s="152" t="s">
+      <c r="F55" s="139"/>
+    </row>
+    <row r="56" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B56" s="142" t="s">
+        <v>89</v>
+      </c>
+      <c r="C56" s="151" t="s">
+        <v>213</v>
+      </c>
+      <c r="D56" s="142"/>
+      <c r="E56" s="143" t="s">
+        <v>212</v>
+      </c>
+      <c r="F56" s="143" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B57" s="142"/>
+      <c r="C57" s="143"/>
+      <c r="D57" s="142"/>
+      <c r="E57" s="143" t="s">
+        <v>215</v>
+      </c>
+      <c r="F57" s="143" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B58" s="142"/>
+      <c r="C58" s="142"/>
+      <c r="D58" s="142"/>
+      <c r="E58" s="143" t="s">
+        <v>218</v>
+      </c>
+      <c r="F58" s="143" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B59" s="142"/>
+      <c r="C59" s="142"/>
+      <c r="D59" s="143" t="s">
+        <v>219</v>
+      </c>
+      <c r="E59" s="142"/>
+      <c r="F59" s="143" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B60" s="142"/>
+      <c r="C60" s="142"/>
+      <c r="D60" s="142"/>
+      <c r="E60" s="143" t="s">
+        <v>95</v>
+      </c>
+      <c r="F60" s="142"/>
+    </row>
+    <row r="61" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B61" s="142"/>
+      <c r="C61" s="142"/>
+      <c r="D61" s="142"/>
+      <c r="E61" s="142" t="s">
+        <v>96</v>
+      </c>
+      <c r="F61" s="142"/>
+    </row>
+    <row r="62" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B62" s="142"/>
+      <c r="C62" s="142"/>
+      <c r="D62" s="142"/>
+      <c r="E62" s="143" t="s">
+        <v>97</v>
+      </c>
+      <c r="F62" s="143" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B63" s="144" t="s">
+        <v>89</v>
+      </c>
+      <c r="C63" s="152" t="s">
+        <v>221</v>
+      </c>
+      <c r="D63" s="145" t="s">
+        <v>222</v>
+      </c>
+      <c r="E63" s="144"/>
+      <c r="F63" s="145" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B64" s="144"/>
+      <c r="C64" s="144"/>
+      <c r="D64" s="144"/>
+      <c r="E64" s="145" t="s">
+        <v>225</v>
+      </c>
+      <c r="F64" s="144"/>
+    </row>
+    <row r="65" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B65" s="144"/>
+      <c r="C65" s="144"/>
+      <c r="D65" s="144"/>
+      <c r="E65" s="145" t="s">
+        <v>226</v>
+      </c>
+      <c r="F65" s="144"/>
+    </row>
+    <row r="66" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B66" s="144"/>
+      <c r="C66" s="144"/>
+      <c r="D66" s="145" t="s">
+        <v>219</v>
+      </c>
+      <c r="E66" s="144"/>
+      <c r="F66" s="145" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B67" s="144"/>
+      <c r="C67" s="144"/>
+      <c r="D67" s="144"/>
+      <c r="E67" s="145" t="s">
+        <v>97</v>
+      </c>
+      <c r="F67" s="145" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" ht="15.75" customHeight="1">
+      <c r="B68" s="144" t="s">
         <v>91</v>
       </c>
-      <c r="C48" s="163" t="s">
-        <v>205</v>
-      </c>
-      <c r="D48" s="153" t="s">
-        <v>105</v>
-      </c>
-      <c r="E48" s="152"/>
-      <c r="F48" s="153" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="49" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B49" s="152"/>
-      <c r="C49" s="152"/>
-      <c r="D49" s="152"/>
-      <c r="E49" s="153" t="s">
-        <v>208</v>
-      </c>
-      <c r="F49" s="153" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="50" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B50" s="152"/>
-      <c r="C50" s="152"/>
-      <c r="D50" s="152"/>
-      <c r="E50" s="153" t="s">
-        <v>231</v>
-      </c>
-      <c r="F50" s="153" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="51" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B51" s="152"/>
-      <c r="C51" s="152"/>
-      <c r="D51" s="152"/>
-      <c r="E51" s="153" t="s">
-        <v>195</v>
-      </c>
-      <c r="F51" s="153"/>
-    </row>
-    <row r="52" spans="2:6" ht="18" customHeight="1">
-      <c r="B52" s="152" t="s">
-        <v>89</v>
-      </c>
-      <c r="C52" s="163" t="s">
-        <v>198</v>
-      </c>
-      <c r="D52" s="154"/>
-      <c r="E52" s="153" t="s">
-        <v>269</v>
-      </c>
-      <c r="F52" s="153" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="53" spans="2:6" ht="18" customHeight="1">
-      <c r="B53" s="152"/>
-      <c r="C53" s="153"/>
-      <c r="D53" s="154"/>
-      <c r="E53" s="153" t="s">
-        <v>270</v>
-      </c>
-      <c r="F53" s="153" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="54" spans="2:6" ht="18" customHeight="1">
-      <c r="B54" s="152"/>
-      <c r="C54" s="153"/>
-      <c r="D54" s="154"/>
-      <c r="E54" s="153" t="s">
-        <v>273</v>
-      </c>
-      <c r="F54" s="153" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="55" spans="2:6" ht="18" customHeight="1">
-      <c r="B55" s="152"/>
-      <c r="C55" s="153"/>
-      <c r="D55" s="154"/>
-      <c r="E55" s="153" t="s">
-        <v>102</v>
-      </c>
-      <c r="F55" s="152"/>
-    </row>
-    <row r="56" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B56" s="155" t="s">
-        <v>89</v>
-      </c>
-      <c r="C56" s="164" t="s">
-        <v>213</v>
-      </c>
-      <c r="D56" s="155"/>
-      <c r="E56" s="156" t="s">
-        <v>212</v>
-      </c>
-      <c r="F56" s="156" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="57" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B57" s="155"/>
-      <c r="C57" s="156"/>
-      <c r="D57" s="155"/>
-      <c r="E57" s="156" t="s">
-        <v>215</v>
-      </c>
-      <c r="F57" s="156" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="58" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B58" s="155"/>
-      <c r="C58" s="155"/>
-      <c r="D58" s="155"/>
-      <c r="E58" s="156" t="s">
-        <v>218</v>
-      </c>
-      <c r="F58" s="156" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="59" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B59" s="155"/>
-      <c r="C59" s="155"/>
-      <c r="D59" s="156" t="s">
-        <v>219</v>
-      </c>
-      <c r="E59" s="155"/>
-      <c r="F59" s="156" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="60" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B60" s="155"/>
-      <c r="C60" s="155"/>
-      <c r="D60" s="155"/>
-      <c r="E60" s="156" t="s">
-        <v>95</v>
-      </c>
-      <c r="F60" s="155"/>
-    </row>
-    <row r="61" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B61" s="155"/>
-      <c r="C61" s="155"/>
-      <c r="D61" s="155"/>
-      <c r="E61" s="155" t="s">
-        <v>96</v>
-      </c>
-      <c r="F61" s="155"/>
-    </row>
-    <row r="62" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B62" s="155"/>
-      <c r="C62" s="155"/>
-      <c r="D62" s="155"/>
-      <c r="E62" s="156" t="s">
-        <v>97</v>
-      </c>
-      <c r="F62" s="156" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="63" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B63" s="157" t="s">
-        <v>89</v>
-      </c>
-      <c r="C63" s="165" t="s">
-        <v>221</v>
-      </c>
-      <c r="D63" s="158" t="s">
-        <v>222</v>
-      </c>
-      <c r="E63" s="157"/>
-      <c r="F63" s="158" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="64" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B64" s="157"/>
-      <c r="C64" s="157"/>
-      <c r="D64" s="157"/>
-      <c r="E64" s="158" t="s">
-        <v>225</v>
-      </c>
-      <c r="F64" s="157"/>
-    </row>
-    <row r="65" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B65" s="157"/>
-      <c r="C65" s="157"/>
-      <c r="D65" s="157"/>
-      <c r="E65" s="158" t="s">
-        <v>226</v>
-      </c>
-      <c r="F65" s="157"/>
-    </row>
-    <row r="66" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B66" s="157"/>
-      <c r="C66" s="157"/>
-      <c r="D66" s="158" t="s">
-        <v>219</v>
-      </c>
-      <c r="E66" s="157"/>
-      <c r="F66" s="158" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="67" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B67" s="157"/>
-      <c r="C67" s="157"/>
-      <c r="D67" s="157"/>
-      <c r="E67" s="158" t="s">
-        <v>97</v>
-      </c>
-      <c r="F67" s="158" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="68" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B68" s="157" t="s">
-        <v>91</v>
-      </c>
-      <c r="C68" s="165" t="s">
+      <c r="C68" s="152" t="s">
         <v>235</v>
       </c>
-      <c r="D68" s="158" t="s">
+      <c r="D68" s="145" t="s">
         <v>237</v>
       </c>
-      <c r="E68" s="157"/>
-      <c r="F68" s="158" t="s">
+      <c r="E68" s="144"/>
+      <c r="F68" s="145" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="69" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B69" s="157"/>
-      <c r="C69" s="157"/>
-      <c r="D69" s="157"/>
-      <c r="E69" s="158" t="s">
+      <c r="B69" s="144"/>
+      <c r="C69" s="144"/>
+      <c r="D69" s="144"/>
+      <c r="E69" s="145" t="s">
         <v>238</v>
       </c>
-      <c r="F69" s="157"/>
+      <c r="F69" s="144"/>
     </row>
     <row r="70" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B70" s="157"/>
-      <c r="C70" s="157"/>
-      <c r="D70" s="157"/>
-      <c r="E70" s="158" t="s">
+      <c r="B70" s="144"/>
+      <c r="C70" s="144"/>
+      <c r="D70" s="144"/>
+      <c r="E70" s="145" t="s">
         <v>239</v>
       </c>
-      <c r="F70" s="157"/>
+      <c r="F70" s="144"/>
     </row>
     <row r="71" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B71" s="157"/>
-      <c r="C71" s="157"/>
-      <c r="D71" s="157"/>
-      <c r="E71" s="158" t="s">
+      <c r="B71" s="144"/>
+      <c r="C71" s="144"/>
+      <c r="D71" s="144"/>
+      <c r="E71" s="145" t="s">
         <v>240</v>
       </c>
-      <c r="F71" s="157"/>
+      <c r="F71" s="144"/>
     </row>
     <row r="103" spans="4:4" ht="15.75" customHeight="1">
       <c r="D103" t="s">
@@ -4413,9 +4413,9 @@
   <sheetViews>
     <sheetView topLeftCell="CI1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="101" width="4.109375" customWidth="1"/>
+    <col min="1" max="101" width="4.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="7:19" ht="21.75" customHeight="1">
@@ -4563,7 +4563,7 @@
       <c r="R9" s="112"/>
       <c r="S9" s="112"/>
     </row>
-    <row r="10" spans="7:19" ht="15.6">
+    <row r="10" spans="7:19">
       <c r="G10" s="34"/>
       <c r="H10" s="35"/>
       <c r="I10" s="35"/>
@@ -4587,13 +4587,13 @@
       <c r="J11" s="112"/>
       <c r="K11" s="112"/>
       <c r="L11" s="112"/>
-      <c r="M11" s="137"/>
-      <c r="N11" s="130"/>
-      <c r="O11" s="130"/>
+      <c r="M11" s="177"/>
+      <c r="N11" s="170"/>
+      <c r="O11" s="170"/>
       <c r="P11" s="112"/>
       <c r="Q11" s="112"/>
-      <c r="R11" s="137"/>
-      <c r="S11" s="138"/>
+      <c r="R11" s="177"/>
+      <c r="S11" s="178"/>
     </row>
     <row r="12" spans="7:19" ht="15">
       <c r="G12" s="38"/>
@@ -4680,7 +4680,7 @@
       <c r="R16" s="40"/>
       <c r="S16" s="41"/>
     </row>
-    <row r="18" spans="7:23" ht="15.6">
+    <row r="18" spans="7:23" ht="15">
       <c r="G18" s="38"/>
       <c r="H18" s="42"/>
       <c r="I18" s="49"/>
@@ -4799,9 +4799,9 @@
       <c r="W23" s="112"/>
     </row>
     <row r="24" spans="7:23" ht="15">
-      <c r="G24" s="136"/>
-      <c r="H24" s="130"/>
-      <c r="I24" s="130"/>
+      <c r="G24" s="176"/>
+      <c r="H24" s="170"/>
+      <c r="I24" s="170"/>
       <c r="J24" s="112"/>
       <c r="K24" s="112"/>
       <c r="L24" s="112"/>
@@ -4837,9 +4837,9 @@
       <c r="W25" s="112"/>
     </row>
     <row r="26" spans="7:23" ht="15">
-      <c r="G26" s="136"/>
-      <c r="H26" s="130"/>
-      <c r="I26" s="130"/>
+      <c r="G26" s="176"/>
+      <c r="H26" s="170"/>
+      <c r="I26" s="170"/>
       <c r="J26" s="112"/>
       <c r="K26" s="112"/>
       <c r="L26" s="112"/>
@@ -4884,14 +4884,14 @@
       <c r="M28" s="112"/>
       <c r="N28" s="112"/>
       <c r="O28" s="112"/>
-      <c r="P28" s="136"/>
-      <c r="Q28" s="130"/>
-      <c r="R28" s="130"/>
+      <c r="P28" s="176"/>
+      <c r="Q28" s="170"/>
+      <c r="R28" s="170"/>
       <c r="S28" s="112"/>
-      <c r="T28" s="136"/>
-      <c r="U28" s="130"/>
-      <c r="V28" s="130"/>
-      <c r="W28" s="130"/>
+      <c r="T28" s="176"/>
+      <c r="U28" s="170"/>
+      <c r="V28" s="170"/>
+      <c r="W28" s="170"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -4915,32 +4915,32 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
-    <col min="2" max="2" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" customWidth="1"/>
-    <col min="5" max="5" width="13.5546875" customWidth="1"/>
-    <col min="6" max="6" width="17.33203125" customWidth="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1"/>
-    <col min="8" max="8" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="20.109375" customWidth="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" customWidth="1"/>
     <col min="12" max="30" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="87" customHeight="1">
       <c r="B1" s="110"/>
-      <c r="C1" s="134" t="s">
+      <c r="C1" s="174" t="s">
         <v>122</v>
       </c>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
+      <c r="D1" s="170"/>
+      <c r="E1" s="170"/>
+      <c r="F1" s="170"/>
+      <c r="G1" s="170"/>
+      <c r="H1" s="170"/>
     </row>
     <row r="2" spans="2:8" ht="12.75" customHeight="1">
       <c r="B2" s="112"/>
@@ -5054,47 +5054,47 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="13" customWidth="1"/>
     <col min="7" max="26" width="17" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="64.5" customHeight="1">
-      <c r="C1" s="139" t="s">
+      <c r="C1" s="179" t="s">
         <v>130</v>
       </c>
-      <c r="D1" s="130"/>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-    </row>
-    <row r="2" spans="2:11" ht="13.2"/>
-    <row r="3" spans="2:11" ht="13.2">
+      <c r="D1" s="170"/>
+      <c r="E1" s="170"/>
+      <c r="F1" s="170"/>
+    </row>
+    <row r="2" spans="2:11" ht="12.75"/>
+    <row r="3" spans="2:11" ht="12.75">
       <c r="B3" s="56" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="13.2">
+    <row r="4" spans="2:11" ht="12.75">
       <c r="B4" s="57"/>
     </row>
-    <row r="5" spans="2:11" ht="13.2">
+    <row r="5" spans="2:11" ht="12.75">
       <c r="B5" s="113"/>
       <c r="C5" s="113"/>
       <c r="D5" s="113"/>
     </row>
-    <row r="6" spans="2:11" ht="13.2">
+    <row r="6" spans="2:11" ht="12.75">
       <c r="B6" s="113"/>
       <c r="C6" s="113"/>
       <c r="D6" s="113"/>
       <c r="E6" s="113"/>
     </row>
-    <row r="7" spans="2:11" ht="26.4">
-      <c r="B7" s="140" t="s">
+    <row r="7" spans="2:11" ht="25.5">
+      <c r="B7" s="180" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="130"/>
+      <c r="C7" s="170"/>
       <c r="G7" s="113" t="s">
         <v>133</v>
       </c>
@@ -5102,7 +5102,7 @@
       <c r="I7" s="113"/>
       <c r="J7" s="113"/>
     </row>
-    <row r="8" spans="2:11" ht="13.2">
+    <row r="8" spans="2:11" ht="12.75">
       <c r="B8" s="113"/>
       <c r="G8" s="113" t="s">
         <v>134</v>
@@ -5110,7 +5110,7 @@
       <c r="H8" s="113"/>
       <c r="I8" s="113"/>
     </row>
-    <row r="9" spans="2:11" ht="13.2">
+    <row r="9" spans="2:11" ht="12.75">
       <c r="B9" s="58" t="s">
         <v>135</v>
       </c>
@@ -5134,7 +5134,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="13.2">
+    <row r="10" spans="2:11" ht="12.75">
       <c r="B10" s="108"/>
       <c r="D10" s="67"/>
       <c r="G10" s="68" t="s">
@@ -5143,7 +5143,7 @@
       <c r="J10" s="113"/>
       <c r="K10" s="111"/>
     </row>
-    <row r="11" spans="2:11" ht="26.4">
+    <row r="11" spans="2:11" ht="25.5">
       <c r="B11" s="64"/>
       <c r="C11" s="65"/>
       <c r="D11" s="66"/>
@@ -5155,7 +5155,7 @@
       </c>
       <c r="K11" s="111"/>
     </row>
-    <row r="12" spans="2:11" ht="13.2">
+    <row r="12" spans="2:11" ht="12.75">
       <c r="B12" s="108"/>
       <c r="D12" s="67"/>
       <c r="G12" s="68" t="s">
@@ -5163,7 +5163,7 @@
       </c>
       <c r="K12" s="111"/>
     </row>
-    <row r="13" spans="2:11" ht="13.2">
+    <row r="13" spans="2:11" ht="12.75">
       <c r="B13" s="108"/>
       <c r="D13" s="67"/>
       <c r="G13" s="68" t="s">
@@ -5187,31 +5187,31 @@
   </sheetPr>
   <dimension ref="B1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="88" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="88" workbookViewId="0">
       <selection activeCell="D16" sqref="D16:H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="38.5546875" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" customWidth="1"/>
-    <col min="4" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="1" max="1" width="56.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
+    <col min="4" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="16.5703125" customWidth="1"/>
     <col min="9" max="9" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" ht="57" customHeight="1">
       <c r="B1" s="115"/>
       <c r="C1" s="116"/>
-      <c r="D1" s="139" t="s">
+      <c r="D1" s="179" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="130"/>
-      <c r="F1" s="130"/>
-      <c r="G1" s="130"/>
-      <c r="H1" s="130"/>
+      <c r="E1" s="170"/>
+      <c r="F1" s="170"/>
+      <c r="G1" s="170"/>
+      <c r="H1" s="170"/>
     </row>
     <row r="2" spans="2:8" ht="12.75" customHeight="1">
       <c r="B2" s="115"/>
@@ -5241,7 +5241,7 @@
       <c r="F4" s="115"/>
       <c r="H4" s="115"/>
     </row>
-    <row r="5" spans="2:8" ht="13.2">
+    <row r="5" spans="2:8" ht="12.75">
       <c r="B5" s="115"/>
       <c r="C5" s="116"/>
       <c r="D5" s="117"/>
@@ -5281,294 +5281,303 @@
     </row>
     <row r="8" spans="2:8" ht="13.5" customHeight="1">
       <c r="C8" s="116"/>
-      <c r="D8" s="174" t="s">
+      <c r="D8" s="158" t="s">
         <v>155</v>
       </c>
-      <c r="E8" s="175" t="s">
-        <v>279</v>
-      </c>
-      <c r="F8" s="176" t="s">
-        <v>284</v>
-      </c>
-      <c r="G8" s="175"/>
-      <c r="H8" s="177"/>
+      <c r="E8" s="159" t="s">
+        <v>278</v>
+      </c>
+      <c r="F8" s="160" t="s">
+        <v>283</v>
+      </c>
+      <c r="G8" s="159"/>
+      <c r="H8" s="185"/>
     </row>
     <row r="9" spans="2:8" ht="14.25" customHeight="1">
       <c r="B9" s="115"/>
       <c r="C9" s="121"/>
-      <c r="D9" s="178" t="s">
+      <c r="D9" s="161" t="s">
         <v>241</v>
       </c>
-      <c r="E9" s="167" t="s">
-        <v>279</v>
-      </c>
-      <c r="F9" s="179" t="s">
-        <v>284</v>
-      </c>
-      <c r="G9" s="180"/>
-      <c r="H9" s="181"/>
+      <c r="E9" s="154" t="s">
+        <v>278</v>
+      </c>
+      <c r="F9" s="162" t="s">
+        <v>283</v>
+      </c>
+      <c r="G9" s="163"/>
+      <c r="H9" s="164"/>
     </row>
     <row r="10" spans="2:8" ht="12.75" customHeight="1">
       <c r="B10" s="113" t="s">
         <v>156</v>
       </c>
       <c r="C10" s="116"/>
-      <c r="D10" s="166" t="s">
+      <c r="D10" s="153" t="s">
         <v>184</v>
       </c>
-      <c r="E10" s="168" t="s">
-        <v>279</v>
-      </c>
-      <c r="F10" s="167" t="s">
-        <v>284</v>
-      </c>
-      <c r="G10" s="168"/>
-      <c r="H10" s="169"/>
+      <c r="E10" s="155" t="s">
+        <v>278</v>
+      </c>
+      <c r="F10" s="154" t="s">
+        <v>283</v>
+      </c>
+      <c r="G10" s="155"/>
+      <c r="H10" s="156"/>
     </row>
     <row r="11" spans="2:8" ht="12.75" customHeight="1">
       <c r="B11" s="56" t="s">
         <v>157</v>
       </c>
       <c r="C11" s="116"/>
-      <c r="D11" s="166" t="s">
+      <c r="D11" s="153" t="s">
+        <v>266</v>
+      </c>
+      <c r="E11" s="154" t="s">
+        <v>278</v>
+      </c>
+      <c r="F11" s="154" t="s">
+        <v>283</v>
+      </c>
+      <c r="G11" s="155"/>
+      <c r="H11" s="156"/>
+    </row>
+    <row r="12" spans="2:8" ht="15.75" customHeight="1">
+      <c r="D12" s="153" t="s">
+        <v>65</v>
+      </c>
+      <c r="E12" s="155" t="s">
+        <v>278</v>
+      </c>
+      <c r="F12" s="154" t="s">
+        <v>283</v>
+      </c>
+      <c r="G12" s="155"/>
+      <c r="H12" s="156"/>
+    </row>
+    <row r="13" spans="2:8" ht="15.75" customHeight="1">
+      <c r="D13" s="153" t="s">
         <v>267</v>
       </c>
-      <c r="E11" s="167" t="s">
+      <c r="E13" s="155" t="s">
+        <v>278</v>
+      </c>
+      <c r="F13" s="154" t="s">
+        <v>283</v>
+      </c>
+      <c r="G13" s="155"/>
+      <c r="H13" s="156"/>
+    </row>
+    <row r="14" spans="2:8" ht="15.75" customHeight="1">
+      <c r="D14" s="153" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="155" t="s">
+        <v>278</v>
+      </c>
+      <c r="F14" s="154" t="s">
+        <v>283</v>
+      </c>
+      <c r="G14" s="155"/>
+      <c r="H14" s="156"/>
+    </row>
+    <row r="15" spans="2:8" ht="15.75" customHeight="1">
+      <c r="D15" s="153" t="s">
+        <v>182</v>
+      </c>
+      <c r="E15" s="154" t="s">
+        <v>278</v>
+      </c>
+      <c r="F15" s="154" t="s">
+        <v>283</v>
+      </c>
+      <c r="G15" s="155"/>
+      <c r="H15" s="156"/>
+    </row>
+    <row r="16" spans="2:8" ht="15.75" customHeight="1">
+      <c r="D16" s="181" t="s">
         <v>279</v>
       </c>
-      <c r="F11" s="167" t="s">
+      <c r="E16" s="182"/>
+      <c r="F16" s="182"/>
+      <c r="G16" s="182"/>
+      <c r="H16" s="183"/>
+    </row>
+    <row r="17" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D17" s="161" t="s">
+        <v>277</v>
+      </c>
+      <c r="E17" s="167" t="s">
+        <v>278</v>
+      </c>
+      <c r="F17" s="157" t="s">
         <v>284</v>
       </c>
-      <c r="G11" s="168"/>
-      <c r="H11" s="169"/>
-    </row>
-    <row r="12" spans="2:8" ht="15.75" customHeight="1">
-      <c r="D12" s="166" t="s">
-        <v>65</v>
-      </c>
-      <c r="E12" s="168" t="s">
-        <v>279</v>
-      </c>
-      <c r="F12" s="167" t="s">
+      <c r="G17" s="155"/>
+      <c r="H17" s="166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D18" s="161" t="s">
+        <v>280</v>
+      </c>
+      <c r="E18" s="167" t="s">
+        <v>278</v>
+      </c>
+      <c r="F18" s="157" t="s">
         <v>284</v>
       </c>
-      <c r="G12" s="168"/>
-      <c r="H12" s="169"/>
-    </row>
-    <row r="13" spans="2:8" ht="15.75" customHeight="1">
-      <c r="D13" s="166" t="s">
-        <v>268</v>
-      </c>
-      <c r="E13" s="168" t="s">
-        <v>279</v>
-      </c>
-      <c r="F13" s="167" t="s">
-        <v>284</v>
-      </c>
-      <c r="G13" s="168"/>
-      <c r="H13" s="169"/>
-    </row>
-    <row r="14" spans="2:8" ht="15.75" customHeight="1">
-      <c r="D14" s="166" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="168" t="s">
-        <v>279</v>
-      </c>
-      <c r="F14" s="167" t="s">
-        <v>284</v>
-      </c>
-      <c r="G14" s="168"/>
-      <c r="H14" s="169"/>
-    </row>
-    <row r="15" spans="2:8" ht="15.75" customHeight="1">
-      <c r="D15" s="166" t="s">
-        <v>182</v>
-      </c>
-      <c r="E15" s="167" t="s">
-        <v>279</v>
-      </c>
-      <c r="F15" s="167" t="s">
-        <v>284</v>
-      </c>
-      <c r="G15" s="168"/>
-      <c r="H15" s="169"/>
-    </row>
-    <row r="16" spans="2:8" ht="15.75" customHeight="1">
-      <c r="D16" s="170" t="s">
-        <v>280</v>
-      </c>
-      <c r="E16" s="171"/>
-      <c r="F16" s="171"/>
-      <c r="G16" s="171"/>
-      <c r="H16" s="172"/>
-    </row>
-    <row r="17" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D17" s="178" t="s">
+      <c r="G18" s="155"/>
+      <c r="H18" s="166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D19" s="161" t="s">
+        <v>281</v>
+      </c>
+      <c r="E19" s="167" t="s">
         <v>278</v>
       </c>
-      <c r="E17" s="184" t="s">
-        <v>279</v>
-      </c>
-      <c r="F17" s="173" t="s">
+      <c r="F19" s="157" t="s">
         <v>285</v>
       </c>
-      <c r="G17" s="168"/>
-      <c r="H17" s="183">
+      <c r="G19" s="155"/>
+      <c r="H19" s="166">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D18" s="178" t="s">
-        <v>281</v>
-      </c>
-      <c r="E18" s="184" t="s">
-        <v>279</v>
-      </c>
-      <c r="F18" s="173" t="s">
+    <row r="20" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D20" s="161" t="s">
+        <v>282</v>
+      </c>
+      <c r="E20" s="167" t="s">
+        <v>278</v>
+      </c>
+      <c r="F20" s="157" t="s">
         <v>285</v>
       </c>
-      <c r="G18" s="168"/>
-      <c r="H18" s="183">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D19" s="178" t="s">
-        <v>282</v>
-      </c>
-      <c r="E19" s="184" t="s">
-        <v>279</v>
-      </c>
-      <c r="F19" s="173" t="s">
+      <c r="G20" s="155"/>
+      <c r="H20" s="168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D21" s="161" t="s">
         <v>286</v>
       </c>
-      <c r="G19" s="168"/>
-      <c r="H19" s="183">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D20" s="178" t="s">
-        <v>283</v>
-      </c>
-      <c r="E20" s="184" t="s">
-        <v>279</v>
-      </c>
-      <c r="F20" s="173" t="s">
-        <v>286</v>
-      </c>
-      <c r="G20" s="168"/>
-      <c r="H20" s="185">
+      <c r="E21" s="165" t="s">
+        <v>287</v>
+      </c>
+      <c r="F21" s="154" t="s">
+        <v>285</v>
+      </c>
+      <c r="G21" s="155"/>
+      <c r="H21" s="168">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D21" s="178" t="s">
+    <row r="22" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D22" s="161" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="165" t="s">
         <v>287</v>
       </c>
-      <c r="E21" s="182" t="s">
+      <c r="F22" s="154" t="s">
         <v>288</v>
       </c>
-      <c r="F21" s="167" t="s">
-        <v>286</v>
-      </c>
-      <c r="G21" s="168"/>
-      <c r="H21" s="185">
+      <c r="G22" s="155"/>
+      <c r="H22" s="168">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D22" s="178" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="182" t="s">
+    <row r="23" spans="4:8" ht="15.75" customHeight="1">
+      <c r="D23" s="161" t="s">
+        <v>73</v>
+      </c>
+      <c r="E23" s="165" t="s">
+        <v>287</v>
+      </c>
+      <c r="F23" s="154" t="s">
         <v>288</v>
       </c>
-      <c r="F22" s="167" t="s">
-        <v>289</v>
-      </c>
-      <c r="G22" s="168"/>
-      <c r="H22" s="185">
+      <c r="G23" s="155"/>
+      <c r="H23" s="168">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D23" s="178" t="s">
-        <v>73</v>
-      </c>
-      <c r="E23" s="182" t="s">
-        <v>288</v>
-      </c>
-      <c r="F23" s="167" t="s">
-        <v>289</v>
-      </c>
-      <c r="G23" s="168"/>
-      <c r="H23" s="185">
-        <v>0</v>
-      </c>
-    </row>
     <row r="24" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D24" s="166"/>
-      <c r="E24" s="168"/>
-      <c r="F24" s="168"/>
-      <c r="G24" s="168"/>
-      <c r="H24" s="169"/>
+      <c r="D24" s="153"/>
+      <c r="E24" s="155"/>
+      <c r="F24" s="155"/>
+      <c r="G24" s="155"/>
+      <c r="H24" s="156"/>
     </row>
     <row r="25" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D25" s="166"/>
-      <c r="E25" s="168"/>
-      <c r="F25" s="168"/>
-      <c r="G25" s="168"/>
-      <c r="H25" s="169"/>
+      <c r="D25" s="153"/>
+      <c r="E25" s="155"/>
+      <c r="F25" s="155"/>
+      <c r="G25" s="155"/>
+      <c r="H25" s="156"/>
     </row>
     <row r="26" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D26" s="166"/>
-      <c r="E26" s="168"/>
-      <c r="F26" s="168"/>
-      <c r="G26" s="168"/>
-      <c r="H26" s="169"/>
+      <c r="D26" s="153"/>
+      <c r="E26" s="155"/>
+      <c r="F26" s="155"/>
+      <c r="G26" s="155"/>
+      <c r="H26" s="156"/>
     </row>
     <row r="27" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D27" s="166"/>
-      <c r="E27" s="168"/>
-      <c r="F27" s="168"/>
-      <c r="G27" s="168"/>
-      <c r="H27" s="169"/>
+      <c r="D27" s="153"/>
+      <c r="E27" s="155"/>
+      <c r="F27" s="155"/>
+      <c r="G27" s="155"/>
+      <c r="H27" s="156"/>
     </row>
     <row r="28" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D28" s="166"/>
-      <c r="E28" s="168"/>
-      <c r="F28" s="168"/>
-      <c r="G28" s="168"/>
-      <c r="H28" s="169"/>
+      <c r="D28" s="153"/>
+      <c r="E28" s="155"/>
+      <c r="F28" s="155"/>
+      <c r="G28" s="155"/>
+      <c r="H28" s="156"/>
     </row>
     <row r="29" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D29" s="166"/>
-      <c r="E29" s="168"/>
-      <c r="F29" s="168"/>
-      <c r="G29" s="168"/>
-      <c r="H29" s="169"/>
+      <c r="D29" s="153"/>
+      <c r="E29" s="155"/>
+      <c r="F29" s="155"/>
+      <c r="G29" s="155"/>
+      <c r="H29" s="156"/>
     </row>
     <row r="30" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D30" s="166"/>
-      <c r="E30" s="168"/>
-      <c r="F30" s="168"/>
-      <c r="G30" s="168"/>
-      <c r="H30" s="169"/>
+      <c r="D30" s="153"/>
+      <c r="E30" s="155"/>
+      <c r="F30" s="155"/>
+      <c r="G30" s="155"/>
+      <c r="H30" s="156"/>
     </row>
     <row r="31" spans="4:8" ht="15.75" customHeight="1">
-      <c r="D31" s="166"/>
-      <c r="E31" s="168"/>
-      <c r="F31" s="168"/>
-      <c r="G31" s="168"/>
-      <c r="H31" s="169"/>
+      <c r="D31" s="153"/>
+      <c r="E31" s="155"/>
+      <c r="F31" s="155"/>
+      <c r="G31" s="155"/>
+      <c r="H31" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D1:H1"/>
     <mergeCell ref="D16:H16"/>
   </mergeCells>
+  <conditionalFormatting sqref="E17:E20">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Flags">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
 </worksheet>
 </file>
@@ -5584,20 +5593,20 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="17.33203125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.88671875" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" customWidth="1"/>
     <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="39.33203125" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="39.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="8.88671875" customWidth="1"/>
-    <col min="7" max="7" width="30.44140625" customWidth="1"/>
-    <col min="8" max="9" width="10.5546875" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" customWidth="1"/>
+    <col min="8" max="9" width="10.5703125" customWidth="1"/>
     <col min="10" max="10" width="29" customWidth="1"/>
-    <col min="11" max="12" width="10.5546875" customWidth="1"/>
+    <col min="11" max="12" width="10.5703125" customWidth="1"/>
     <col min="13" max="13" width="29" customWidth="1"/>
-    <col min="14" max="23" width="11.44140625" customWidth="1"/>
+    <col min="14" max="23" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:13" ht="21.75" customHeight="1">
@@ -5622,12 +5631,12 @@
       <c r="E3" s="71"/>
       <c r="F3" s="71"/>
       <c r="G3" s="71"/>
-      <c r="H3" s="141"/>
-      <c r="I3" s="130"/>
-      <c r="J3" s="130"/>
-      <c r="K3" s="130"/>
-      <c r="L3" s="130"/>
-      <c r="M3" s="130"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="170"/>
+      <c r="J3" s="170"/>
+      <c r="K3" s="170"/>
+      <c r="L3" s="170"/>
+      <c r="M3" s="170"/>
     </row>
     <row r="4" spans="2:13" ht="21.75" customHeight="1">
       <c r="B4" s="102"/>

</xml_diff>